<commit_message>
Add sum test case
</commit_message>
<xml_diff>
--- a/JobSolutions_Testcase_v2.2.xlsx
+++ b/JobSolutions_Testcase_v2.2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="16" r:id="rId1"/>
@@ -638,7 +638,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="101">
   <si>
     <t>Online ID</t>
   </si>
@@ -680,9 +680,6 @@
   </si>
   <si>
     <t xml:space="preserve">Total </t>
-  </si>
-  <si>
-    <t>System Test</t>
   </si>
   <si>
     <t>Number of Testcase</t>
@@ -1472,7 +1469,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1525,12 +1522,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1734,12 +1725,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1798,6 +1783,12 @@
     <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1822,12 +1813,6 @@
     <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1848,6 +1833,33 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2227,8 +2239,8 @@
   </sheetPr>
   <dimension ref="A1:AI44"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:G11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="14.25"/>
@@ -2267,13 +2279,13 @@
       <c r="S2" s="13"/>
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
-      <c r="V2" s="73"/>
+      <c r="V2" s="71"/>
       <c r="W2" s="13"/>
       <c r="X2" s="14"/>
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="5"/>
@@ -2287,7 +2299,7 @@
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
-      <c r="N3" s="72"/>
+      <c r="N3" s="70"/>
       <c r="O3" s="18"/>
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
@@ -2295,7 +2307,7 @@
       <c r="S3" s="18"/>
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
-      <c r="V3" s="74"/>
+      <c r="V3" s="72"/>
       <c r="W3" s="18"/>
       <c r="X3" s="19"/>
     </row>
@@ -2354,13 +2366,13 @@
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
-      <c r="O6" s="124" t="s">
+      <c r="O6" s="120" t="s">
         <v>7</v>
       </c>
-      <c r="P6" s="124"/>
-      <c r="Q6" s="124"/>
-      <c r="R6" s="124"/>
-      <c r="S6" s="124"/>
+      <c r="P6" s="120"/>
+      <c r="Q6" s="120"/>
+      <c r="R6" s="120"/>
+      <c r="S6" s="120"/>
       <c r="U6" s="18"/>
       <c r="V6" s="18"/>
       <c r="W6" s="18"/>
@@ -2370,11 +2382,11 @@
       <c r="B7" s="22"/>
       <c r="E7" s="4"/>
       <c r="G7" s="21"/>
-      <c r="O7" s="124"/>
-      <c r="P7" s="124"/>
-      <c r="Q7" s="124"/>
-      <c r="R7" s="124"/>
-      <c r="S7" s="124"/>
+      <c r="O7" s="120"/>
+      <c r="P7" s="120"/>
+      <c r="Q7" s="120"/>
+      <c r="R7" s="120"/>
+      <c r="S7" s="120"/>
       <c r="X7" s="23"/>
     </row>
     <row r="8" spans="1:24" s="24" customFormat="1" ht="14.25" customHeight="1">
@@ -2383,7 +2395,7 @@
       <c r="J8" s="29"/>
       <c r="K8" s="29"/>
       <c r="L8" s="31"/>
-      <c r="X8" s="71"/>
+      <c r="X8" s="69"/>
     </row>
     <row r="9" spans="1:24" ht="14.25" customHeight="1">
       <c r="B9" s="30"/>
@@ -2392,11 +2404,11 @@
         <v>8</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
-      <c r="H9" s="76"/>
+      <c r="H9" s="74"/>
       <c r="X9" s="19"/>
     </row>
     <row r="10" spans="1:24" ht="14.25" customHeight="1">
@@ -2408,19 +2420,19 @@
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
-      <c r="H10" s="76"/>
+      <c r="H10" s="74"/>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
-      <c r="L10" s="117" t="s">
-        <v>16</v>
+      <c r="L10" s="113" t="s">
+        <v>15</v>
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="21"/>
       <c r="Q10" s="21"/>
       <c r="R10" s="21"/>
       <c r="S10" s="21"/>
-      <c r="V10" s="45"/>
+      <c r="V10" s="43"/>
       <c r="X10" s="19"/>
     </row>
     <row r="11" spans="1:24" ht="14.25" customHeight="1">
@@ -2429,13 +2441,13 @@
       <c r="D11" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="125">
+      <c r="E11" s="121">
         <f ca="1">TODAY()</f>
         <v>43443</v>
       </c>
-      <c r="F11" s="125"/>
-      <c r="G11" s="125"/>
-      <c r="H11" s="76"/>
+      <c r="F11" s="121"/>
+      <c r="G11" s="121"/>
+      <c r="H11" s="74"/>
       <c r="L11" s="33" t="s">
         <v>11</v>
       </c>
@@ -2446,11 +2458,11 @@
       </c>
       <c r="P11" s="33"/>
       <c r="Q11" s="33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R11" s="33"/>
       <c r="S11" s="33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T11" s="33"/>
       <c r="U11" s="33" t="s">
@@ -2461,28 +2473,28 @@
     </row>
     <row r="12" spans="1:24">
       <c r="B12" s="30"/>
-      <c r="L12" s="34" t="s">
-        <v>14</v>
+      <c r="L12" s="34">
+        <v>1</v>
       </c>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
-      <c r="O12" s="67">
-        <v>2</v>
-      </c>
-      <c r="P12" s="67"/>
-      <c r="Q12" s="68">
+      <c r="O12" s="65">
+        <v>0</v>
+      </c>
+      <c r="P12" s="65"/>
+      <c r="Q12" s="66">
         <v>3</v>
       </c>
-      <c r="R12" s="68"/>
-      <c r="S12" s="69">
-        <v>4</v>
-      </c>
-      <c r="T12" s="69"/>
-      <c r="U12" s="70">
+      <c r="R12" s="66"/>
+      <c r="S12" s="67">
+        <v>0</v>
+      </c>
+      <c r="T12" s="67"/>
+      <c r="U12" s="68">
         <f t="shared" ref="U12:U18" si="0">SUM(O12:T12)</f>
-        <v>9</v>
-      </c>
-      <c r="V12" s="70"/>
+        <v>3</v>
+      </c>
+      <c r="V12" s="68"/>
       <c r="X12" s="19"/>
     </row>
     <row r="13" spans="1:24">
@@ -2492,23 +2504,23 @@
       </c>
       <c r="M13" s="34"/>
       <c r="N13" s="34"/>
-      <c r="O13" s="67">
-        <v>22</v>
-      </c>
-      <c r="P13" s="67"/>
-      <c r="Q13" s="68">
-        <v>22</v>
-      </c>
-      <c r="R13" s="68"/>
-      <c r="S13" s="69">
-        <v>22</v>
-      </c>
-      <c r="T13" s="69"/>
-      <c r="U13" s="70">
+      <c r="O13" s="65">
+        <v>0</v>
+      </c>
+      <c r="P13" s="65"/>
+      <c r="Q13" s="66">
+        <v>1</v>
+      </c>
+      <c r="R13" s="66"/>
+      <c r="S13" s="67">
+        <v>0</v>
+      </c>
+      <c r="T13" s="67"/>
+      <c r="U13" s="68">
         <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="V13" s="70"/>
+        <v>1</v>
+      </c>
+      <c r="V13" s="68"/>
       <c r="X13" s="19"/>
     </row>
     <row r="14" spans="1:24">
@@ -2518,184 +2530,162 @@
       </c>
       <c r="M14" s="35"/>
       <c r="N14" s="35"/>
-      <c r="O14" s="67">
-        <v>32</v>
-      </c>
-      <c r="P14" s="67"/>
-      <c r="Q14" s="68">
-        <v>32</v>
-      </c>
-      <c r="R14" s="68"/>
-      <c r="S14" s="69">
-        <v>32</v>
-      </c>
-      <c r="T14" s="69"/>
-      <c r="U14" s="70">
+      <c r="O14" s="65">
+        <v>0</v>
+      </c>
+      <c r="P14" s="65"/>
+      <c r="Q14" s="66">
+        <v>1</v>
+      </c>
+      <c r="R14" s="66"/>
+      <c r="S14" s="67">
+        <v>1</v>
+      </c>
+      <c r="T14" s="67"/>
+      <c r="U14" s="68">
         <f t="shared" si="0"/>
-        <v>96</v>
-      </c>
-      <c r="V14" s="70"/>
+        <v>2</v>
+      </c>
+      <c r="V14" s="68"/>
       <c r="X14" s="19"/>
     </row>
     <row r="15" spans="1:24">
       <c r="B15" s="30"/>
       <c r="D15" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="75"/>
+        <v>32</v>
+      </c>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
       <c r="L15" s="34">
         <v>4</v>
       </c>
       <c r="M15" s="34"/>
       <c r="N15" s="34"/>
-      <c r="O15" s="67">
-        <v>42</v>
-      </c>
-      <c r="P15" s="67"/>
-      <c r="Q15" s="68">
-        <v>42</v>
-      </c>
-      <c r="R15" s="68"/>
-      <c r="S15" s="69">
-        <v>42</v>
-      </c>
-      <c r="T15" s="69"/>
-      <c r="U15" s="70">
+      <c r="O15" s="65">
+        <v>0</v>
+      </c>
+      <c r="P15" s="65"/>
+      <c r="Q15" s="66">
+        <v>2</v>
+      </c>
+      <c r="R15" s="66"/>
+      <c r="S15" s="67">
+        <v>1</v>
+      </c>
+      <c r="T15" s="67"/>
+      <c r="U15" s="68">
         <f t="shared" si="0"/>
-        <v>126</v>
-      </c>
-      <c r="V15" s="70"/>
+        <v>3</v>
+      </c>
+      <c r="V15" s="68"/>
       <c r="X15" s="19"/>
     </row>
     <row r="16" spans="1:24">
       <c r="B16" s="30"/>
       <c r="D16" s="18"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
       <c r="L16" s="35">
         <v>5</v>
       </c>
       <c r="M16" s="35"/>
       <c r="N16" s="35"/>
-      <c r="O16" s="67">
-        <v>52</v>
-      </c>
-      <c r="P16" s="67"/>
-      <c r="Q16" s="68">
-        <v>52</v>
-      </c>
-      <c r="R16" s="68"/>
-      <c r="S16" s="69">
-        <v>52</v>
-      </c>
-      <c r="T16" s="69"/>
-      <c r="U16" s="70">
+      <c r="O16" s="65">
+        <v>0</v>
+      </c>
+      <c r="P16" s="65"/>
+      <c r="Q16" s="66">
+        <v>1</v>
+      </c>
+      <c r="R16" s="66"/>
+      <c r="S16" s="67">
+        <v>0</v>
+      </c>
+      <c r="T16" s="67"/>
+      <c r="U16" s="68">
         <f t="shared" si="0"/>
-        <v>156</v>
-      </c>
-      <c r="V16" s="70"/>
+        <v>1</v>
+      </c>
+      <c r="V16" s="68"/>
       <c r="X16" s="19"/>
     </row>
     <row r="17" spans="2:35">
       <c r="B17" s="30"/>
       <c r="D17" s="18"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="L17" s="34">
-        <v>6</v>
-      </c>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="67">
-        <v>62</v>
-      </c>
-      <c r="P17" s="67"/>
-      <c r="Q17" s="68">
-        <v>62</v>
-      </c>
-      <c r="R17" s="68"/>
-      <c r="S17" s="69">
-        <v>62</v>
-      </c>
-      <c r="T17" s="69"/>
-      <c r="U17" s="70">
-        <f t="shared" si="0"/>
-        <v>186</v>
-      </c>
-      <c r="V17" s="70"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="L17" s="149" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="150"/>
+      <c r="N17" s="150"/>
+      <c r="O17" s="151">
+        <f>SUM(O10:O16)</f>
+        <v>0</v>
+      </c>
+      <c r="P17" s="151"/>
+      <c r="Q17" s="151">
+        <f>SUM(Q10:Q16)</f>
+        <v>8</v>
+      </c>
+      <c r="R17" s="151"/>
+      <c r="S17" s="151">
+        <f>SUM(S10:S16)</f>
+        <v>2</v>
+      </c>
+      <c r="T17" s="151"/>
+      <c r="U17" s="152">
+        <f>SUM(U10:U16)</f>
+        <v>10</v>
+      </c>
+      <c r="V17" s="152"/>
       <c r="X17" s="19"/>
     </row>
     <row r="18" spans="2:35">
       <c r="B18" s="30"/>
       <c r="D18" s="18"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="L18" s="35">
-        <v>7</v>
-      </c>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="67">
-        <v>72</v>
-      </c>
-      <c r="P18" s="67"/>
-      <c r="Q18" s="68">
-        <v>72</v>
-      </c>
-      <c r="R18" s="68"/>
-      <c r="S18" s="69">
-        <v>72</v>
-      </c>
-      <c r="T18" s="69"/>
-      <c r="U18" s="70">
-        <f t="shared" si="0"/>
-        <v>216</v>
-      </c>
-      <c r="V18" s="70"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="L18" s="153"/>
+      <c r="M18" s="153"/>
+      <c r="N18" s="153"/>
+      <c r="O18" s="154"/>
+      <c r="P18" s="154"/>
+      <c r="Q18" s="154"/>
+      <c r="R18" s="154"/>
+      <c r="S18" s="154"/>
+      <c r="T18" s="154"/>
+      <c r="U18" s="154"/>
+      <c r="V18" s="154"/>
       <c r="X18" s="19"/>
     </row>
     <row r="19" spans="2:35">
       <c r="B19" s="30"/>
       <c r="D19" s="18"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="L19" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="115">
-        <f>SUM(O12:O18)</f>
-        <v>284</v>
-      </c>
-      <c r="P19" s="115"/>
-      <c r="Q19" s="115">
-        <f>SUM(Q12:Q18)</f>
-        <v>285</v>
-      </c>
-      <c r="R19" s="115"/>
-      <c r="S19" s="115">
-        <f>SUM(S12:S18)</f>
-        <v>286</v>
-      </c>
-      <c r="T19" s="115"/>
-      <c r="U19" s="116">
-        <f>SUM(U12:U18)</f>
-        <v>855</v>
-      </c>
-      <c r="V19" s="116"/>
-      <c r="W19" s="78"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="L19" s="155"/>
+      <c r="M19" s="153"/>
+      <c r="N19" s="153"/>
+      <c r="O19" s="156"/>
+      <c r="P19" s="156"/>
+      <c r="Q19" s="156"/>
+      <c r="R19" s="156"/>
+      <c r="S19" s="156"/>
+      <c r="T19" s="156"/>
+      <c r="U19" s="157"/>
+      <c r="V19" s="157"/>
+      <c r="W19" s="76"/>
       <c r="X19" s="19"/>
     </row>
     <row r="20" spans="2:35">
@@ -2710,8 +2700,8 @@
       <c r="S20" s="17"/>
       <c r="T20" s="17"/>
       <c r="U20" s="17"/>
-      <c r="V20" s="45"/>
-      <c r="W20" s="45"/>
+      <c r="V20" s="43"/>
+      <c r="W20" s="43"/>
       <c r="X20" s="19"/>
     </row>
     <row r="21" spans="2:35">
@@ -2723,126 +2713,126 @@
       <c r="B22" s="15"/>
       <c r="C22" s="4"/>
       <c r="D22" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="75"/>
+        <v>33</v>
+      </c>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
       <c r="W22" s="17"/>
       <c r="X22" s="23"/>
     </row>
     <row r="23" spans="2:35" s="17" customFormat="1">
       <c r="B23" s="22"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="W23" s="79"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="W23" s="77"/>
       <c r="X23" s="23"/>
     </row>
     <row r="24" spans="2:35" s="17" customFormat="1">
       <c r="B24" s="22"/>
       <c r="D24" s="18"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
-      <c r="L24" s="117" t="s">
-        <v>46</v>
-      </c>
-      <c r="M24" s="107"/>
-      <c r="N24" s="107"/>
-      <c r="O24" s="107"/>
-      <c r="P24" s="108"/>
-      <c r="Q24" s="108"/>
-      <c r="R24" s="108"/>
-      <c r="S24" s="108"/>
-      <c r="T24" s="108"/>
-      <c r="U24" s="108"/>
-      <c r="V24" s="108"/>
-      <c r="W24" s="77"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="L24" s="113" t="s">
+        <v>45</v>
+      </c>
+      <c r="M24" s="105"/>
+      <c r="N24" s="105"/>
+      <c r="O24" s="105"/>
+      <c r="P24" s="106"/>
+      <c r="Q24" s="106"/>
+      <c r="R24" s="106"/>
+      <c r="S24" s="106"/>
+      <c r="T24" s="106"/>
+      <c r="U24" s="106"/>
+      <c r="V24" s="106"/>
+      <c r="W24" s="75"/>
       <c r="X24" s="23"/>
     </row>
     <row r="25" spans="2:35" s="17" customFormat="1">
       <c r="B25" s="22"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="L25" s="109"/>
-      <c r="M25" s="110"/>
-      <c r="N25" s="110"/>
-      <c r="O25" s="110"/>
-      <c r="P25" s="111"/>
-      <c r="Q25" s="111"/>
-      <c r="R25" s="111"/>
-      <c r="S25" s="111"/>
-      <c r="T25" s="111"/>
-      <c r="U25" s="111"/>
-      <c r="V25" s="111"/>
-      <c r="W25" s="77"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="L25" s="107"/>
+      <c r="M25" s="108"/>
+      <c r="N25" s="108"/>
+      <c r="O25" s="108"/>
+      <c r="P25" s="109"/>
+      <c r="Q25" s="109"/>
+      <c r="R25" s="109"/>
+      <c r="S25" s="109"/>
+      <c r="T25" s="109"/>
+      <c r="U25" s="109"/>
+      <c r="V25" s="109"/>
+      <c r="W25" s="75"/>
       <c r="X25" s="23"/>
     </row>
     <row r="26" spans="2:35" s="17" customFormat="1">
       <c r="B26" s="22"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="44"/>
-      <c r="L26" s="109"/>
-      <c r="M26" s="110"/>
-      <c r="N26" s="110"/>
-      <c r="O26" s="110"/>
-      <c r="P26" s="111"/>
-      <c r="Q26" s="111"/>
-      <c r="R26" s="111"/>
-      <c r="S26" s="111"/>
-      <c r="T26" s="111"/>
-      <c r="U26" s="111"/>
-      <c r="V26" s="111"/>
-      <c r="W26" s="77"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="L26" s="107"/>
+      <c r="M26" s="108"/>
+      <c r="N26" s="108"/>
+      <c r="O26" s="108"/>
+      <c r="P26" s="109"/>
+      <c r="Q26" s="109"/>
+      <c r="R26" s="109"/>
+      <c r="S26" s="109"/>
+      <c r="T26" s="109"/>
+      <c r="U26" s="109"/>
+      <c r="V26" s="109"/>
+      <c r="W26" s="75"/>
       <c r="X26" s="23"/>
-      <c r="AB26" s="80"/>
+      <c r="AB26" s="78"/>
     </row>
     <row r="27" spans="2:35" s="17" customFormat="1">
       <c r="B27" s="22"/>
-      <c r="D27" s="38"/>
+      <c r="D27" s="36"/>
       <c r="E27" s="4"/>
-      <c r="L27" s="109"/>
-      <c r="M27" s="110"/>
-      <c r="N27" s="110"/>
-      <c r="O27" s="110"/>
-      <c r="P27" s="111"/>
-      <c r="Q27" s="111"/>
-      <c r="R27" s="111"/>
-      <c r="S27" s="111"/>
-      <c r="T27" s="111"/>
-      <c r="U27" s="111"/>
-      <c r="V27" s="111"/>
-      <c r="W27" s="77"/>
+      <c r="L27" s="107"/>
+      <c r="M27" s="108"/>
+      <c r="N27" s="108"/>
+      <c r="O27" s="108"/>
+      <c r="P27" s="109"/>
+      <c r="Q27" s="109"/>
+      <c r="R27" s="109"/>
+      <c r="S27" s="109"/>
+      <c r="T27" s="109"/>
+      <c r="U27" s="109"/>
+      <c r="V27" s="109"/>
+      <c r="W27" s="75"/>
       <c r="X27" s="23"/>
-      <c r="AB27" s="80"/>
+      <c r="AB27" s="78"/>
     </row>
     <row r="28" spans="2:35" s="17" customFormat="1">
       <c r="B28" s="22"/>
-      <c r="D28" s="38"/>
+      <c r="D28" s="36"/>
       <c r="E28" s="4"/>
-      <c r="L28" s="109"/>
-      <c r="M28" s="110"/>
-      <c r="N28" s="110"/>
-      <c r="O28" s="110"/>
-      <c r="P28" s="111"/>
-      <c r="Q28" s="111"/>
-      <c r="R28" s="111"/>
-      <c r="S28" s="111"/>
-      <c r="T28" s="111"/>
-      <c r="U28" s="111"/>
-      <c r="V28" s="111"/>
-      <c r="W28" s="77"/>
+      <c r="L28" s="107"/>
+      <c r="M28" s="108"/>
+      <c r="N28" s="108"/>
+      <c r="O28" s="108"/>
+      <c r="P28" s="109"/>
+      <c r="Q28" s="109"/>
+      <c r="R28" s="109"/>
+      <c r="S28" s="109"/>
+      <c r="T28" s="109"/>
+      <c r="U28" s="109"/>
+      <c r="V28" s="109"/>
+      <c r="W28" s="75"/>
       <c r="X28" s="23"/>
-      <c r="AB28" s="80"/>
+      <c r="AB28" s="78"/>
     </row>
     <row r="29" spans="2:35" s="17" customFormat="1">
       <c r="B29" s="22"/>
@@ -2852,40 +2842,40 @@
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
       <c r="K29" s="31"/>
-      <c r="L29" s="109"/>
-      <c r="M29" s="110"/>
-      <c r="N29" s="110"/>
-      <c r="O29" s="110"/>
-      <c r="P29" s="111"/>
-      <c r="Q29" s="111"/>
-      <c r="R29" s="111"/>
-      <c r="S29" s="111"/>
-      <c r="T29" s="111"/>
-      <c r="U29" s="111"/>
-      <c r="V29" s="111"/>
-      <c r="W29" s="77"/>
+      <c r="L29" s="107"/>
+      <c r="M29" s="108"/>
+      <c r="N29" s="108"/>
+      <c r="O29" s="108"/>
+      <c r="P29" s="109"/>
+      <c r="Q29" s="109"/>
+      <c r="R29" s="109"/>
+      <c r="S29" s="109"/>
+      <c r="T29" s="109"/>
+      <c r="U29" s="109"/>
+      <c r="V29" s="109"/>
+      <c r="W29" s="75"/>
       <c r="X29" s="23"/>
     </row>
     <row r="30" spans="2:35" s="17" customFormat="1">
       <c r="B30" s="22"/>
-      <c r="L30" s="109"/>
-      <c r="M30" s="110"/>
-      <c r="N30" s="110"/>
-      <c r="O30" s="110"/>
-      <c r="P30" s="111"/>
-      <c r="Q30" s="111"/>
-      <c r="R30" s="111"/>
-      <c r="S30" s="111"/>
-      <c r="T30" s="111"/>
-      <c r="U30" s="111"/>
-      <c r="V30" s="111"/>
-      <c r="W30" s="77"/>
+      <c r="L30" s="107"/>
+      <c r="M30" s="108"/>
+      <c r="N30" s="108"/>
+      <c r="O30" s="108"/>
+      <c r="P30" s="109"/>
+      <c r="Q30" s="109"/>
+      <c r="R30" s="109"/>
+      <c r="S30" s="109"/>
+      <c r="T30" s="109"/>
+      <c r="U30" s="109"/>
+      <c r="V30" s="109"/>
+      <c r="W30" s="75"/>
       <c r="X30" s="23"/>
     </row>
     <row r="31" spans="2:35">
       <c r="B31" s="15"/>
-      <c r="C31" s="39" t="s">
-        <v>17</v>
+      <c r="C31" s="37" t="s">
+        <v>16</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="28"/>
@@ -2895,18 +2885,18 @@
       <c r="I31" s="18"/>
       <c r="J31" s="18"/>
       <c r="K31" s="18"/>
-      <c r="L31" s="112"/>
-      <c r="M31" s="110"/>
-      <c r="N31" s="110"/>
-      <c r="O31" s="110"/>
-      <c r="P31" s="111"/>
-      <c r="Q31" s="111"/>
-      <c r="R31" s="111"/>
-      <c r="S31" s="111"/>
-      <c r="T31" s="111"/>
-      <c r="U31" s="111"/>
-      <c r="V31" s="111"/>
-      <c r="W31" s="77"/>
+      <c r="L31" s="110"/>
+      <c r="M31" s="108"/>
+      <c r="N31" s="108"/>
+      <c r="O31" s="108"/>
+      <c r="P31" s="109"/>
+      <c r="Q31" s="109"/>
+      <c r="R31" s="109"/>
+      <c r="S31" s="109"/>
+      <c r="T31" s="109"/>
+      <c r="U31" s="109"/>
+      <c r="V31" s="109"/>
+      <c r="W31" s="75"/>
       <c r="X31" s="23"/>
       <c r="AA31" s="17"/>
       <c r="AB31" s="17"/>
@@ -2919,9 +2909,9 @@
       <c r="AI31" s="17"/>
     </row>
     <row r="32" spans="2:35">
-      <c r="B32" s="46"/>
-      <c r="C32" s="40" t="s">
-        <v>18</v>
+      <c r="B32" s="44"/>
+      <c r="C32" s="38" t="s">
+        <v>17</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -2931,18 +2921,18 @@
       <c r="I32" s="18"/>
       <c r="J32" s="18"/>
       <c r="K32" s="18"/>
-      <c r="L32" s="109"/>
-      <c r="M32" s="110"/>
-      <c r="N32" s="110"/>
-      <c r="O32" s="110"/>
-      <c r="P32" s="111"/>
-      <c r="Q32" s="111"/>
-      <c r="R32" s="111"/>
-      <c r="S32" s="111"/>
-      <c r="T32" s="111"/>
-      <c r="U32" s="111"/>
-      <c r="V32" s="111"/>
-      <c r="W32" s="77"/>
+      <c r="L32" s="107"/>
+      <c r="M32" s="108"/>
+      <c r="N32" s="108"/>
+      <c r="O32" s="108"/>
+      <c r="P32" s="109"/>
+      <c r="Q32" s="109"/>
+      <c r="R32" s="109"/>
+      <c r="S32" s="109"/>
+      <c r="T32" s="109"/>
+      <c r="U32" s="109"/>
+      <c r="V32" s="109"/>
+      <c r="W32" s="75"/>
       <c r="X32" s="23"/>
       <c r="AA32" s="17"/>
       <c r="AB32" s="17"/>
@@ -2955,7 +2945,7 @@
       <c r="AI32" s="17"/>
     </row>
     <row r="33" spans="1:35">
-      <c r="B33" s="46"/>
+      <c r="B33" s="44"/>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -2965,18 +2955,18 @@
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
       <c r="K33" s="18"/>
-      <c r="L33" s="109"/>
-      <c r="M33" s="113"/>
-      <c r="N33" s="110"/>
-      <c r="O33" s="110"/>
-      <c r="P33" s="111"/>
-      <c r="Q33" s="111"/>
-      <c r="R33" s="111"/>
-      <c r="S33" s="111"/>
-      <c r="T33" s="111"/>
-      <c r="U33" s="111"/>
-      <c r="V33" s="114"/>
-      <c r="W33" s="78"/>
+      <c r="L33" s="107"/>
+      <c r="M33" s="111"/>
+      <c r="N33" s="108"/>
+      <c r="O33" s="108"/>
+      <c r="P33" s="109"/>
+      <c r="Q33" s="109"/>
+      <c r="R33" s="109"/>
+      <c r="S33" s="109"/>
+      <c r="T33" s="109"/>
+      <c r="U33" s="109"/>
+      <c r="V33" s="112"/>
+      <c r="W33" s="76"/>
       <c r="X33" s="23"/>
       <c r="AA33" s="17"/>
       <c r="AB33" s="17"/>
@@ -2990,8 +2980,8 @@
     </row>
     <row r="34" spans="1:35">
       <c r="B34" s="30"/>
-      <c r="C34" s="39" t="s">
-        <v>19</v>
+      <c r="C34" s="37" t="s">
+        <v>18</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="28"/>
@@ -3011,11 +3001,11 @@
       <c r="S34" s="17"/>
       <c r="T34" s="17"/>
       <c r="U34" s="17"/>
-      <c r="V34" s="45"/>
-      <c r="W34" s="45"/>
+      <c r="V34" s="43"/>
+      <c r="W34" s="43"/>
       <c r="X34" s="23"/>
       <c r="AA34" s="17"/>
-      <c r="AB34" s="80"/>
+      <c r="AB34" s="78"/>
       <c r="AC34" s="17"/>
       <c r="AD34" s="17"/>
       <c r="AE34" s="17"/>
@@ -3026,8 +3016,8 @@
     </row>
     <row r="35" spans="1:35">
       <c r="B35" s="30"/>
-      <c r="C35" s="40" t="s">
-        <v>18</v>
+      <c r="C35" s="38" t="s">
+        <v>17</v>
       </c>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
@@ -3058,29 +3048,29 @@
       <c r="AI35" s="17"/>
     </row>
     <row r="36" spans="1:35" ht="5.25" customHeight="1">
-      <c r="B36" s="41"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="42"/>
-      <c r="K36" s="42"/>
-      <c r="L36" s="42"/>
-      <c r="M36" s="42"/>
-      <c r="N36" s="42"/>
-      <c r="O36" s="42"/>
-      <c r="P36" s="42"/>
-      <c r="Q36" s="42"/>
-      <c r="R36" s="42"/>
-      <c r="S36" s="42"/>
-      <c r="T36" s="42"/>
-      <c r="U36" s="42"/>
-      <c r="V36" s="42"/>
-      <c r="W36" s="42"/>
-      <c r="X36" s="43"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="40"/>
+      <c r="N36" s="40"/>
+      <c r="O36" s="40"/>
+      <c r="P36" s="40"/>
+      <c r="Q36" s="40"/>
+      <c r="R36" s="40"/>
+      <c r="S36" s="40"/>
+      <c r="T36" s="40"/>
+      <c r="U36" s="40"/>
+      <c r="V36" s="40"/>
+      <c r="W36" s="40"/>
+      <c r="X36" s="41"/>
       <c r="AA36" s="17"/>
       <c r="AB36" s="17"/>
       <c r="AC36" s="17"/>
@@ -3294,8 +3284,8 @@
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A61" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A52" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -3307,1588 +3297,1588 @@
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="62" customFormat="1">
-      <c r="A1" s="81" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="82" t="str">
+    <row r="1" spans="1:11" s="60" customFormat="1">
+      <c r="A1" s="79" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="80" t="str">
         <f>Overview!E9</f>
         <v xml:space="preserve">Job Solutions </v>
       </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="84" t="s">
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="82" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="85" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="104">
+      <c r="I1" s="102">
         <f ca="1">COUNTIF(H1:H778,"OK")</f>
         <v>8</v>
       </c>
-      <c r="J1" s="86" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" s="87"/>
-    </row>
-    <row r="2" spans="1:11" s="62" customFormat="1">
-      <c r="A2" s="119" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="89" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="92" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="105">
+      <c r="J1" s="84" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="85"/>
+    </row>
+    <row r="2" spans="1:11" s="60" customFormat="1">
+      <c r="A2" s="115" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="87" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="90" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="103">
         <f ca="1">COUNTIF(H2:H779,"Not OK")</f>
         <v>2</v>
       </c>
-      <c r="J2" s="93" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" s="94"/>
-    </row>
-    <row r="3" spans="1:11" s="62" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A3" s="88" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="89" t="s">
+      <c r="J2" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="92"/>
+    </row>
+    <row r="3" spans="1:11" s="60" customFormat="1" ht="11.25" customHeight="1">
+      <c r="A3" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="92" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="106">
+      <c r="B3" s="87" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="90" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="104">
         <f ca="1">COUNTIF(H2:H779,"Untested")</f>
         <v>0</v>
       </c>
-      <c r="J3" s="93" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="94"/>
-    </row>
-    <row r="4" spans="1:11" s="62" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A4" s="95"/>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="96" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="89"/>
-      <c r="I4" s="105">
+      <c r="J3" s="91" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="92"/>
+    </row>
+    <row r="4" spans="1:11" s="60" customFormat="1" ht="11.25" customHeight="1">
+      <c r="A4" s="93"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="94" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="87"/>
+      <c r="I4" s="103">
         <f ca="1">COUNTIF(H3:H780,"Result")</f>
         <v>10</v>
       </c>
-      <c r="J4" s="93"/>
-      <c r="K4" s="94"/>
-    </row>
-    <row r="5" spans="1:11" s="62" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A5" s="97"/>
-      <c r="B5" s="98"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="101"/>
-      <c r="K5" s="102"/>
-    </row>
-    <row r="6" spans="1:11" s="62" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A6" s="63"/>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="92"/>
+    </row>
+    <row r="5" spans="1:11" s="60" customFormat="1" ht="11.25" customHeight="1">
+      <c r="A5" s="95"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="96"/>
+      <c r="J5" s="99"/>
+      <c r="K5" s="100"/>
+    </row>
+    <row r="6" spans="1:11" s="60" customFormat="1" ht="11.25" customHeight="1">
+      <c r="A6" s="61"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
     </row>
     <row r="7" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="126" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="126"/>
-      <c r="D7" s="126"/>
-      <c r="E7" s="126"/>
-      <c r="F7" s="126"/>
-      <c r="G7" s="126"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
-      <c r="J7" s="126"/>
-      <c r="K7" s="126"/>
+      <c r="B7" s="122" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="122"/>
+      <c r="I7" s="122"/>
+      <c r="J7" s="122"/>
+      <c r="K7" s="122"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="125" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="129" t="s">
+      <c r="C8" s="126"/>
+      <c r="D8" s="125" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="126"/>
+      <c r="F8" s="125" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="130"/>
-      <c r="D8" s="129" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="130"/>
-      <c r="F8" s="129" t="s">
+      <c r="G8" s="126"/>
+      <c r="H8" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="130"/>
-      <c r="H8" s="128" t="s">
+      <c r="I8" s="124"/>
+      <c r="J8" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="128"/>
-      <c r="J8" s="48" t="s">
+      <c r="K8" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="49" t="s">
+    </row>
+    <row r="9" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A9" s="48">
+        <v>1</v>
+      </c>
+      <c r="B9" s="142" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="143"/>
+      <c r="D9" s="134" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="135"/>
+      <c r="F9" s="134" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="135"/>
+      <c r="H9" s="132" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="133"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="129"/>
+    </row>
+    <row r="10" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A10" s="45" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A9" s="50">
+      <c r="B10" s="144"/>
+      <c r="C10" s="145"/>
+      <c r="D10" s="136"/>
+      <c r="E10" s="137"/>
+      <c r="F10" s="136"/>
+      <c r="G10" s="137"/>
+      <c r="H10" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="146" t="s">
+      <c r="J10" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="130"/>
+    </row>
+    <row r="11" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A11" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="144"/>
+      <c r="C11" s="145"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="137"/>
+      <c r="F11" s="136"/>
+      <c r="G11" s="137"/>
+      <c r="H11" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="147"/>
-      <c r="D9" s="136" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="137"/>
-      <c r="F9" s="136" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="137"/>
-      <c r="H9" s="144" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" s="145"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="133"/>
-    </row>
-    <row r="10" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A10" s="47" t="s">
+      <c r="I11" s="50"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="130"/>
+    </row>
+    <row r="12" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A12" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="144"/>
+      <c r="C12" s="145"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="137"/>
+      <c r="F12" s="136"/>
+      <c r="G12" s="137"/>
+      <c r="H12" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="148"/>
-      <c r="C10" s="149"/>
-      <c r="D10" s="138"/>
-      <c r="E10" s="139"/>
-      <c r="F10" s="138"/>
-      <c r="G10" s="139"/>
-      <c r="H10" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="K10" s="134"/>
-    </row>
-    <row r="11" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A11" s="51" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="148"/>
-      <c r="C11" s="149"/>
-      <c r="D11" s="138"/>
-      <c r="E11" s="139"/>
-      <c r="F11" s="138"/>
-      <c r="G11" s="139"/>
-      <c r="H11" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="I11" s="52"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="134"/>
-    </row>
-    <row r="12" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A12" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="148"/>
-      <c r="C12" s="149"/>
-      <c r="D12" s="138"/>
-      <c r="E12" s="139"/>
-      <c r="F12" s="138"/>
-      <c r="G12" s="139"/>
-      <c r="H12" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="J12" s="47"/>
-      <c r="K12" s="134"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="130"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A13" s="53">
+      <c r="A13" s="51">
         <v>981</v>
       </c>
-      <c r="B13" s="150"/>
-      <c r="C13" s="151"/>
-      <c r="D13" s="140"/>
-      <c r="E13" s="141"/>
-      <c r="F13" s="140"/>
-      <c r="G13" s="141"/>
-      <c r="H13" s="55">
+      <c r="B13" s="146"/>
+      <c r="C13" s="147"/>
+      <c r="D13" s="138"/>
+      <c r="E13" s="139"/>
+      <c r="F13" s="138"/>
+      <c r="G13" s="139"/>
+      <c r="H13" s="53">
         <f ca="1">TODAY()</f>
         <v>43443</v>
       </c>
-      <c r="I13" s="55"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="135"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="131"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A14" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="131" t="s">
+      <c r="A14" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="132"/>
-      <c r="D14" s="131" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="132"/>
-      <c r="F14" s="131" t="s">
+      <c r="C14" s="128"/>
+      <c r="D14" s="127" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="128"/>
+      <c r="F14" s="127" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="128"/>
+      <c r="H14" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="132"/>
-      <c r="H14" s="152" t="s">
+      <c r="I14" s="148"/>
+      <c r="J14" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="152"/>
-      <c r="J14" s="59" t="s">
+      <c r="K14" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="K14" s="58" t="s">
+    </row>
+    <row r="15" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A15" s="48">
+        <v>2</v>
+      </c>
+      <c r="B15" s="142" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="143"/>
+      <c r="D15" s="134" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="135"/>
+      <c r="F15" s="134" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="135"/>
+      <c r="H15" s="140" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="141"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="129"/>
+    </row>
+    <row r="16" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A16" s="57" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A15" s="50">
-        <v>2</v>
-      </c>
-      <c r="B15" s="146" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="147"/>
-      <c r="D15" s="136" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="137"/>
-      <c r="F15" s="136" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" s="137"/>
-      <c r="H15" s="142" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="143"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="133"/>
-    </row>
-    <row r="16" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A16" s="59" t="s">
+      <c r="B16" s="144"/>
+      <c r="C16" s="145"/>
+      <c r="D16" s="136"/>
+      <c r="E16" s="137"/>
+      <c r="F16" s="136"/>
+      <c r="G16" s="137"/>
+      <c r="H16" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" s="130"/>
+    </row>
+    <row r="17" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A17" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="144"/>
+      <c r="C17" s="145"/>
+      <c r="D17" s="136"/>
+      <c r="E17" s="137"/>
+      <c r="F17" s="136"/>
+      <c r="G17" s="137"/>
+      <c r="H17" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="50"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="130"/>
+    </row>
+    <row r="18" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A18" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="144"/>
+      <c r="C18" s="145"/>
+      <c r="D18" s="136"/>
+      <c r="E18" s="137"/>
+      <c r="F18" s="136"/>
+      <c r="G18" s="137"/>
+      <c r="H18" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="148"/>
-      <c r="C16" s="149"/>
-      <c r="D16" s="138"/>
-      <c r="E16" s="139"/>
-      <c r="F16" s="138"/>
-      <c r="G16" s="139"/>
-      <c r="H16" s="59" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="J16" s="59" t="s">
-        <v>31</v>
-      </c>
-      <c r="K16" s="134"/>
-    </row>
-    <row r="17" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A17" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="148"/>
-      <c r="C17" s="149"/>
-      <c r="D17" s="138"/>
-      <c r="E17" s="139"/>
-      <c r="F17" s="138"/>
-      <c r="G17" s="139"/>
-      <c r="H17" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="I17" s="52"/>
-      <c r="J17" s="50"/>
-      <c r="K17" s="134"/>
-    </row>
-    <row r="18" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A18" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="148"/>
-      <c r="C18" s="149"/>
-      <c r="D18" s="138"/>
-      <c r="E18" s="139"/>
-      <c r="F18" s="138"/>
-      <c r="G18" s="139"/>
-      <c r="H18" s="59" t="s">
-        <v>30</v>
-      </c>
-      <c r="I18" s="59" t="s">
-        <v>27</v>
-      </c>
-      <c r="J18" s="59"/>
-      <c r="K18" s="134"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="130"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A19" s="53">
+      <c r="A19" s="51">
         <v>921</v>
       </c>
-      <c r="B19" s="150"/>
-      <c r="C19" s="151"/>
-      <c r="D19" s="140"/>
-      <c r="E19" s="141"/>
-      <c r="F19" s="140"/>
-      <c r="G19" s="141"/>
-      <c r="H19" s="55">
+      <c r="B19" s="146"/>
+      <c r="C19" s="147"/>
+      <c r="D19" s="138"/>
+      <c r="E19" s="139"/>
+      <c r="F19" s="138"/>
+      <c r="G19" s="139"/>
+      <c r="H19" s="53">
         <f ca="1">TODAY()</f>
         <v>43443</v>
       </c>
-      <c r="I19" s="52"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="134"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="130"/>
     </row>
     <row r="20" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="125" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="129" t="s">
+      <c r="C20" s="126"/>
+      <c r="D20" s="125" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="126"/>
+      <c r="F20" s="125" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="130"/>
-      <c r="D20" s="129" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="130"/>
-      <c r="F20" s="129" t="s">
+      <c r="G20" s="126"/>
+      <c r="H20" s="123" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="130"/>
-      <c r="H20" s="127" t="s">
+      <c r="I20" s="123"/>
+      <c r="J20" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="I20" s="127"/>
-      <c r="J20" s="47" t="s">
+      <c r="K20" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="K20" s="60" t="s">
+    </row>
+    <row r="21" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A21" s="48">
+        <v>3</v>
+      </c>
+      <c r="B21" s="142" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="143"/>
+      <c r="D21" s="134" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="135"/>
+      <c r="F21" s="134" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="135"/>
+      <c r="H21" s="140" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="141"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="129"/>
+    </row>
+    <row r="22" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A22" s="45" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A21" s="50">
-        <v>3</v>
-      </c>
-      <c r="B21" s="146" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="147"/>
-      <c r="D21" s="136" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" s="137"/>
-      <c r="F21" s="136" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" s="137"/>
-      <c r="H21" s="142" t="s">
-        <v>32</v>
-      </c>
-      <c r="I21" s="143"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="133"/>
-    </row>
-    <row r="22" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A22" s="47" t="s">
+      <c r="B22" s="144"/>
+      <c r="C22" s="145"/>
+      <c r="D22" s="136"/>
+      <c r="E22" s="137"/>
+      <c r="F22" s="136"/>
+      <c r="G22" s="137"/>
+      <c r="H22" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="K22" s="130"/>
+    </row>
+    <row r="23" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A23" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="144"/>
+      <c r="C23" s="145"/>
+      <c r="D23" s="136"/>
+      <c r="E23" s="137"/>
+      <c r="F23" s="136"/>
+      <c r="G23" s="137"/>
+      <c r="H23" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" s="50"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="130"/>
+    </row>
+    <row r="24" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A24" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="144"/>
+      <c r="C24" s="145"/>
+      <c r="D24" s="136"/>
+      <c r="E24" s="137"/>
+      <c r="F24" s="136"/>
+      <c r="G24" s="137"/>
+      <c r="H24" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="148"/>
-      <c r="C22" s="149"/>
-      <c r="D22" s="138"/>
-      <c r="E22" s="139"/>
-      <c r="F22" s="138"/>
-      <c r="G22" s="139"/>
-      <c r="H22" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="J22" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="K22" s="134"/>
-    </row>
-    <row r="23" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A23" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="148"/>
-      <c r="C23" s="149"/>
-      <c r="D23" s="138"/>
-      <c r="E23" s="139"/>
-      <c r="F23" s="138"/>
-      <c r="G23" s="139"/>
-      <c r="H23" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="I23" s="52"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="134"/>
-    </row>
-    <row r="24" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A24" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="148"/>
-      <c r="C24" s="149"/>
-      <c r="D24" s="138"/>
-      <c r="E24" s="139"/>
-      <c r="F24" s="138"/>
-      <c r="G24" s="139"/>
-      <c r="H24" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="I24" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="J24" s="47"/>
-      <c r="K24" s="134"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="130"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A25" s="53">
+      <c r="A25" s="51">
         <v>823</v>
       </c>
-      <c r="B25" s="150"/>
-      <c r="C25" s="151"/>
-      <c r="D25" s="140"/>
-      <c r="E25" s="141"/>
-      <c r="F25" s="140"/>
-      <c r="G25" s="141"/>
-      <c r="H25" s="55">
+      <c r="B25" s="146"/>
+      <c r="C25" s="147"/>
+      <c r="D25" s="138"/>
+      <c r="E25" s="139"/>
+      <c r="F25" s="138"/>
+      <c r="G25" s="139"/>
+      <c r="H25" s="53">
         <f ca="1">TODAY()</f>
         <v>43443</v>
       </c>
-      <c r="I25" s="52"/>
-      <c r="J25" s="50"/>
-      <c r="K25" s="135"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="131"/>
     </row>
     <row r="26" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A26" s="103" t="s">
+      <c r="A26" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="126" t="s">
+      <c r="B26" s="122" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="122"/>
+      <c r="D26" s="122"/>
+      <c r="E26" s="122"/>
+      <c r="F26" s="122"/>
+      <c r="G26" s="122"/>
+      <c r="H26" s="122"/>
+      <c r="I26" s="122"/>
+      <c r="J26" s="122"/>
+      <c r="K26" s="122"/>
+    </row>
+    <row r="27" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A27" s="116" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="127" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="128"/>
+      <c r="D27" s="127" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="128"/>
+      <c r="F27" s="127" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" s="128"/>
+      <c r="H27" s="148" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="148"/>
+      <c r="J27" s="116" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" s="116" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A28" s="48">
+        <v>4</v>
+      </c>
+      <c r="B28" s="142" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="126"/>
-      <c r="D26" s="126"/>
-      <c r="E26" s="126"/>
-      <c r="F26" s="126"/>
-      <c r="G26" s="126"/>
-      <c r="H26" s="126"/>
-      <c r="I26" s="126"/>
-      <c r="J26" s="126"/>
-      <c r="K26" s="126"/>
-    </row>
-    <row r="27" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A27" s="120" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="131" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="132"/>
-      <c r="D27" s="131" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="132"/>
-      <c r="F27" s="131" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="132"/>
-      <c r="H27" s="152" t="s">
-        <v>23</v>
-      </c>
-      <c r="I27" s="152"/>
-      <c r="J27" s="120" t="s">
-        <v>24</v>
-      </c>
-      <c r="K27" s="120" t="s">
+      <c r="C28" s="143"/>
+      <c r="D28" s="134" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="135"/>
+      <c r="F28" s="134" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="135"/>
+      <c r="H28" s="132" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="133"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="129"/>
+    </row>
+    <row r="29" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A29" s="116" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A28" s="50">
-        <v>4</v>
-      </c>
-      <c r="B28" s="146" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="147"/>
-      <c r="D28" s="136" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="137"/>
-      <c r="F28" s="136" t="s">
-        <v>67</v>
-      </c>
-      <c r="G28" s="137"/>
-      <c r="H28" s="144" t="s">
-        <v>32</v>
-      </c>
-      <c r="I28" s="145"/>
-      <c r="J28" s="50"/>
-      <c r="K28" s="133"/>
-    </row>
-    <row r="29" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A29" s="120" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="148"/>
-      <c r="C29" s="149"/>
-      <c r="D29" s="138"/>
-      <c r="E29" s="139"/>
-      <c r="F29" s="138"/>
-      <c r="G29" s="139"/>
-      <c r="H29" s="120" t="s">
-        <v>28</v>
-      </c>
-      <c r="I29" s="120" t="s">
+      <c r="B29" s="144"/>
+      <c r="C29" s="145"/>
+      <c r="D29" s="136"/>
+      <c r="E29" s="137"/>
+      <c r="F29" s="136"/>
+      <c r="G29" s="137"/>
+      <c r="H29" s="116" t="s">
+        <v>27</v>
+      </c>
+      <c r="I29" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="J29" s="120" t="s">
-        <v>31</v>
-      </c>
-      <c r="K29" s="134"/>
+      <c r="J29" s="116" t="s">
+        <v>30</v>
+      </c>
+      <c r="K29" s="130"/>
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A30" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30" s="148"/>
-      <c r="C30" s="149"/>
-      <c r="D30" s="138"/>
-      <c r="E30" s="139"/>
-      <c r="F30" s="138"/>
-      <c r="G30" s="139"/>
-      <c r="H30" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="I30" s="52"/>
-      <c r="J30" s="50"/>
-      <c r="K30" s="134"/>
+      <c r="A30" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="144"/>
+      <c r="C30" s="145"/>
+      <c r="D30" s="136"/>
+      <c r="E30" s="137"/>
+      <c r="F30" s="136"/>
+      <c r="G30" s="137"/>
+      <c r="H30" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="I30" s="50"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="130"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A31" s="120" t="s">
+      <c r="A31" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="148"/>
-      <c r="C31" s="149"/>
-      <c r="D31" s="138"/>
-      <c r="E31" s="139"/>
-      <c r="F31" s="138"/>
-      <c r="G31" s="139"/>
-      <c r="H31" s="120" t="s">
-        <v>30</v>
-      </c>
-      <c r="I31" s="120"/>
-      <c r="J31" s="120"/>
-      <c r="K31" s="134"/>
+      <c r="B31" s="144"/>
+      <c r="C31" s="145"/>
+      <c r="D31" s="136"/>
+      <c r="E31" s="137"/>
+      <c r="F31" s="136"/>
+      <c r="G31" s="137"/>
+      <c r="H31" s="116" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31" s="116"/>
+      <c r="J31" s="116"/>
+      <c r="K31" s="130"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A32" s="53">
-        <v>922</v>
-      </c>
-      <c r="B32" s="150"/>
-      <c r="C32" s="151"/>
-      <c r="D32" s="140"/>
-      <c r="E32" s="141"/>
-      <c r="F32" s="140"/>
-      <c r="G32" s="141"/>
-      <c r="H32" s="55">
+      <c r="A32" s="51">
+        <v>785</v>
+      </c>
+      <c r="B32" s="146"/>
+      <c r="C32" s="147"/>
+      <c r="D32" s="138"/>
+      <c r="E32" s="139"/>
+      <c r="F32" s="138"/>
+      <c r="G32" s="139"/>
+      <c r="H32" s="53">
         <f ca="1">TODAY()</f>
         <v>43443</v>
       </c>
-      <c r="I32" s="52"/>
-      <c r="J32" s="50"/>
-      <c r="K32" s="135"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="131"/>
     </row>
     <row r="33" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A33" s="103" t="s">
+      <c r="A33" s="101" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="122" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="126" t="s">
+      <c r="C33" s="122"/>
+      <c r="D33" s="122"/>
+      <c r="E33" s="122"/>
+      <c r="F33" s="122"/>
+      <c r="G33" s="122"/>
+      <c r="H33" s="122"/>
+      <c r="I33" s="122"/>
+      <c r="J33" s="122"/>
+      <c r="K33" s="122"/>
+    </row>
+    <row r="34" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A34" s="118" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="125" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="126"/>
+      <c r="D34" s="125" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="126"/>
+      <c r="F34" s="125" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="126"/>
+      <c r="H34" s="123" t="s">
+        <v>22</v>
+      </c>
+      <c r="I34" s="123"/>
+      <c r="J34" s="118" t="s">
+        <v>23</v>
+      </c>
+      <c r="K34" s="117" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A35" s="48">
+        <v>5</v>
+      </c>
+      <c r="B35" s="142" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="126"/>
-      <c r="D33" s="126"/>
-      <c r="E33" s="126"/>
-      <c r="F33" s="126"/>
-      <c r="G33" s="126"/>
-      <c r="H33" s="126"/>
-      <c r="I33" s="126"/>
-      <c r="J33" s="126"/>
-      <c r="K33" s="126"/>
-    </row>
-    <row r="34" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A34" s="122" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" s="129" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="130"/>
-      <c r="D34" s="129" t="s">
-        <v>49</v>
-      </c>
-      <c r="E34" s="130"/>
-      <c r="F34" s="129" t="s">
-        <v>22</v>
-      </c>
-      <c r="G34" s="130"/>
-      <c r="H34" s="127" t="s">
-        <v>23</v>
-      </c>
-      <c r="I34" s="127"/>
-      <c r="J34" s="122" t="s">
-        <v>24</v>
-      </c>
-      <c r="K34" s="121" t="s">
+      <c r="C35" s="143"/>
+      <c r="D35" s="134" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" s="135"/>
+      <c r="F35" s="134" t="s">
+        <v>71</v>
+      </c>
+      <c r="G35" s="135"/>
+      <c r="H35" s="140" t="s">
+        <v>28</v>
+      </c>
+      <c r="I35" s="141"/>
+      <c r="J35" s="52" t="s">
+        <v>73</v>
+      </c>
+      <c r="K35" s="129"/>
+    </row>
+    <row r="36" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A36" s="118" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A35" s="50">
-        <v>5</v>
-      </c>
-      <c r="B35" s="146" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="147"/>
-      <c r="D35" s="136" t="s">
-        <v>71</v>
-      </c>
-      <c r="E35" s="137"/>
-      <c r="F35" s="136" t="s">
+      <c r="B36" s="144"/>
+      <c r="C36" s="145"/>
+      <c r="D36" s="136"/>
+      <c r="E36" s="137"/>
+      <c r="F36" s="136"/>
+      <c r="G36" s="137"/>
+      <c r="H36" s="118" t="s">
+        <v>27</v>
+      </c>
+      <c r="I36" s="118" t="s">
+        <v>1</v>
+      </c>
+      <c r="J36" s="118" t="s">
+        <v>30</v>
+      </c>
+      <c r="K36" s="130"/>
+    </row>
+    <row r="37" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A37" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="144"/>
+      <c r="C37" s="145"/>
+      <c r="D37" s="136"/>
+      <c r="E37" s="137"/>
+      <c r="F37" s="136"/>
+      <c r="G37" s="137"/>
+      <c r="H37" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="I37" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="G35" s="137"/>
-      <c r="H35" s="142" t="s">
+      <c r="J37" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="K37" s="130"/>
+    </row>
+    <row r="38" spans="1:11" ht="10.5" customHeight="1">
+      <c r="A38" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="144"/>
+      <c r="C38" s="145"/>
+      <c r="D38" s="136"/>
+      <c r="E38" s="137"/>
+      <c r="F38" s="136"/>
+      <c r="G38" s="137"/>
+      <c r="H38" s="118" t="s">
         <v>29</v>
       </c>
-      <c r="I35" s="143"/>
-      <c r="J35" s="54" t="s">
-        <v>74</v>
-      </c>
-      <c r="K35" s="133"/>
-    </row>
-    <row r="36" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A36" s="122" t="s">
+      <c r="I38" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="148"/>
-      <c r="C36" s="149"/>
-      <c r="D36" s="138"/>
-      <c r="E36" s="139"/>
-      <c r="F36" s="138"/>
-      <c r="G36" s="139"/>
-      <c r="H36" s="122" t="s">
-        <v>28</v>
-      </c>
-      <c r="I36" s="122" t="s">
-        <v>1</v>
-      </c>
-      <c r="J36" s="122" t="s">
-        <v>31</v>
-      </c>
-      <c r="K36" s="134"/>
-    </row>
-    <row r="37" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A37" s="51" t="s">
-        <v>96</v>
-      </c>
-      <c r="B37" s="148"/>
-      <c r="C37" s="149"/>
-      <c r="D37" s="138"/>
-      <c r="E37" s="139"/>
-      <c r="F37" s="138"/>
-      <c r="G37" s="139"/>
-      <c r="H37" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="I37" s="52" t="s">
-        <v>73</v>
-      </c>
-      <c r="J37" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="K37" s="134"/>
-    </row>
-    <row r="38" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A38" s="122" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="148"/>
-      <c r="C38" s="149"/>
-      <c r="D38" s="138"/>
-      <c r="E38" s="139"/>
-      <c r="F38" s="138"/>
-      <c r="G38" s="139"/>
-      <c r="H38" s="122" t="s">
-        <v>30</v>
-      </c>
-      <c r="I38" s="122" t="s">
-        <v>27</v>
-      </c>
-      <c r="J38" s="122"/>
-      <c r="K38" s="134"/>
+      <c r="J38" s="118"/>
+      <c r="K38" s="130"/>
     </row>
     <row r="39" spans="1:11" ht="10.5" customHeight="1">
-      <c r="A39" s="53">
-        <v>823</v>
-      </c>
-      <c r="B39" s="150"/>
-      <c r="C39" s="151"/>
-      <c r="D39" s="140"/>
-      <c r="E39" s="141"/>
-      <c r="F39" s="140"/>
-      <c r="G39" s="141"/>
-      <c r="H39" s="55">
+      <c r="A39" s="51">
+        <v>678</v>
+      </c>
+      <c r="B39" s="146"/>
+      <c r="C39" s="147"/>
+      <c r="D39" s="138"/>
+      <c r="E39" s="139"/>
+      <c r="F39" s="138"/>
+      <c r="G39" s="139"/>
+      <c r="H39" s="53">
         <f ca="1">TODAY()</f>
         <v>43443</v>
       </c>
-      <c r="I39" s="52">
+      <c r="I39" s="50">
         <v>43446</v>
       </c>
-      <c r="J39" s="50"/>
-      <c r="K39" s="135"/>
-    </row>
-    <row r="40" spans="1:11" s="62" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A40" s="123" t="s">
-        <v>20</v>
-      </c>
-      <c r="B40" s="131" t="s">
+      <c r="J39" s="48"/>
+      <c r="K39" s="131"/>
+    </row>
+    <row r="40" spans="1:11" s="60" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A40" s="119" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="C40" s="132"/>
-      <c r="D40" s="131" t="s">
-        <v>49</v>
-      </c>
-      <c r="E40" s="132"/>
-      <c r="F40" s="131" t="s">
+      <c r="C40" s="128"/>
+      <c r="D40" s="127" t="s">
+        <v>48</v>
+      </c>
+      <c r="E40" s="128"/>
+      <c r="F40" s="127" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" s="128"/>
+      <c r="H40" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="G40" s="132"/>
-      <c r="H40" s="152" t="s">
+      <c r="I40" s="148"/>
+      <c r="J40" s="119" t="s">
         <v>23</v>
       </c>
-      <c r="I40" s="152"/>
-      <c r="J40" s="123" t="s">
+      <c r="K40" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="K40" s="123" t="s">
+    </row>
+    <row r="41" spans="1:11" s="60" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A41" s="48">
+        <v>6</v>
+      </c>
+      <c r="B41" s="142" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="143"/>
+      <c r="D41" s="134" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="135"/>
+      <c r="F41" s="134" t="s">
+        <v>77</v>
+      </c>
+      <c r="G41" s="135"/>
+      <c r="H41" s="132" t="s">
+        <v>31</v>
+      </c>
+      <c r="I41" s="133"/>
+      <c r="J41" s="48"/>
+      <c r="K41" s="129"/>
+    </row>
+    <row r="42" spans="1:11" s="60" customFormat="1">
+      <c r="A42" s="119" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" s="62" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A41" s="50">
-        <v>6</v>
-      </c>
-      <c r="B41" s="146" t="s">
-        <v>76</v>
-      </c>
-      <c r="C41" s="147"/>
-      <c r="D41" s="136" t="s">
-        <v>77</v>
-      </c>
-      <c r="E41" s="137"/>
-      <c r="F41" s="136" t="s">
-        <v>78</v>
-      </c>
-      <c r="G41" s="137"/>
-      <c r="H41" s="144" t="s">
-        <v>32</v>
-      </c>
-      <c r="I41" s="145"/>
-      <c r="J41" s="50"/>
-      <c r="K41" s="133"/>
-    </row>
-    <row r="42" spans="1:11" s="62" customFormat="1">
-      <c r="A42" s="123" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="148"/>
-      <c r="C42" s="149"/>
-      <c r="D42" s="138"/>
-      <c r="E42" s="139"/>
-      <c r="F42" s="138"/>
-      <c r="G42" s="139"/>
-      <c r="H42" s="123" t="s">
-        <v>28</v>
-      </c>
-      <c r="I42" s="123" t="s">
+      <c r="B42" s="144"/>
+      <c r="C42" s="145"/>
+      <c r="D42" s="136"/>
+      <c r="E42" s="137"/>
+      <c r="F42" s="136"/>
+      <c r="G42" s="137"/>
+      <c r="H42" s="119" t="s">
+        <v>27</v>
+      </c>
+      <c r="I42" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="J42" s="123" t="s">
-        <v>31</v>
-      </c>
-      <c r="K42" s="134"/>
-    </row>
-    <row r="43" spans="1:11" s="62" customFormat="1">
-      <c r="A43" s="51" t="s">
-        <v>95</v>
-      </c>
-      <c r="B43" s="148"/>
-      <c r="C43" s="149"/>
-      <c r="D43" s="138"/>
-      <c r="E43" s="139"/>
-      <c r="F43" s="138"/>
-      <c r="G43" s="139"/>
-      <c r="H43" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="I43" s="52"/>
-      <c r="J43" s="50"/>
-      <c r="K43" s="134"/>
-    </row>
-    <row r="44" spans="1:11" s="62" customFormat="1">
-      <c r="A44" s="123" t="s">
+      <c r="J42" s="119" t="s">
+        <v>30</v>
+      </c>
+      <c r="K42" s="130"/>
+    </row>
+    <row r="43" spans="1:11" s="60" customFormat="1">
+      <c r="A43" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" s="144"/>
+      <c r="C43" s="145"/>
+      <c r="D43" s="136"/>
+      <c r="E43" s="137"/>
+      <c r="F43" s="136"/>
+      <c r="G43" s="137"/>
+      <c r="H43" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="I43" s="50"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="130"/>
+    </row>
+    <row r="44" spans="1:11" s="60" customFormat="1">
+      <c r="A44" s="119" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="148"/>
-      <c r="C44" s="149"/>
-      <c r="D44" s="138"/>
-      <c r="E44" s="139"/>
-      <c r="F44" s="138"/>
-      <c r="G44" s="139"/>
-      <c r="H44" s="123" t="s">
-        <v>30</v>
-      </c>
-      <c r="I44" s="123"/>
-      <c r="J44" s="123"/>
-      <c r="K44" s="134"/>
-    </row>
-    <row r="45" spans="1:11" s="62" customFormat="1">
-      <c r="A45" s="53">
-        <v>922</v>
-      </c>
-      <c r="B45" s="150"/>
-      <c r="C45" s="151"/>
-      <c r="D45" s="140"/>
-      <c r="E45" s="141"/>
-      <c r="F45" s="140"/>
-      <c r="G45" s="141"/>
-      <c r="H45" s="55">
+      <c r="B44" s="144"/>
+      <c r="C44" s="145"/>
+      <c r="D44" s="136"/>
+      <c r="E44" s="137"/>
+      <c r="F44" s="136"/>
+      <c r="G44" s="137"/>
+      <c r="H44" s="119" t="s">
+        <v>29</v>
+      </c>
+      <c r="I44" s="119"/>
+      <c r="J44" s="119"/>
+      <c r="K44" s="130"/>
+    </row>
+    <row r="45" spans="1:11" s="60" customFormat="1">
+      <c r="A45" s="51">
+        <v>980</v>
+      </c>
+      <c r="B45" s="146"/>
+      <c r="C45" s="147"/>
+      <c r="D45" s="138"/>
+      <c r="E45" s="139"/>
+      <c r="F45" s="138"/>
+      <c r="G45" s="139"/>
+      <c r="H45" s="53">
         <f ca="1">TODAY()</f>
         <v>43443</v>
       </c>
-      <c r="I45" s="52"/>
-      <c r="J45" s="50"/>
-      <c r="K45" s="135"/>
-    </row>
-    <row r="46" spans="1:11" s="62" customFormat="1">
-      <c r="A46" s="103" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" s="126" t="s">
+      <c r="I45" s="50"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="131"/>
+    </row>
+    <row r="46" spans="1:11" s="60" customFormat="1">
+      <c r="A46" s="101" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" s="122" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="122"/>
+      <c r="D46" s="122"/>
+      <c r="E46" s="122"/>
+      <c r="F46" s="122"/>
+      <c r="G46" s="122"/>
+      <c r="H46" s="122"/>
+      <c r="I46" s="122"/>
+      <c r="J46" s="122"/>
+      <c r="K46" s="122"/>
+    </row>
+    <row r="47" spans="1:11" s="60" customFormat="1">
+      <c r="A47" s="118" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="125" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" s="126"/>
+      <c r="D47" s="125" t="s">
+        <v>48</v>
+      </c>
+      <c r="E47" s="126"/>
+      <c r="F47" s="125" t="s">
+        <v>21</v>
+      </c>
+      <c r="G47" s="126"/>
+      <c r="H47" s="123" t="s">
+        <v>22</v>
+      </c>
+      <c r="I47" s="123"/>
+      <c r="J47" s="118" t="s">
+        <v>23</v>
+      </c>
+      <c r="K47" s="117" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="60" customFormat="1">
+      <c r="A48" s="48">
+        <v>7</v>
+      </c>
+      <c r="B48" s="142" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="126"/>
-      <c r="D46" s="126"/>
-      <c r="E46" s="126"/>
-      <c r="F46" s="126"/>
-      <c r="G46" s="126"/>
-      <c r="H46" s="126"/>
-      <c r="I46" s="126"/>
-      <c r="J46" s="126"/>
-      <c r="K46" s="126"/>
-    </row>
-    <row r="47" spans="1:11" s="62" customFormat="1">
-      <c r="A47" s="122" t="s">
-        <v>20</v>
-      </c>
-      <c r="B47" s="129" t="s">
-        <v>21</v>
-      </c>
-      <c r="C47" s="130"/>
-      <c r="D47" s="129" t="s">
-        <v>49</v>
-      </c>
-      <c r="E47" s="130"/>
-      <c r="F47" s="129" t="s">
-        <v>22</v>
-      </c>
-      <c r="G47" s="130"/>
-      <c r="H47" s="127" t="s">
-        <v>23</v>
-      </c>
-      <c r="I47" s="127"/>
-      <c r="J47" s="122" t="s">
-        <v>24</v>
-      </c>
-      <c r="K47" s="121" t="s">
+      <c r="C48" s="143"/>
+      <c r="D48" s="134" t="s">
+        <v>80</v>
+      </c>
+      <c r="E48" s="135"/>
+      <c r="F48" s="134" t="s">
+        <v>81</v>
+      </c>
+      <c r="G48" s="135"/>
+      <c r="H48" s="140" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" s="141"/>
+      <c r="J48" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="K48" s="129"/>
+    </row>
+    <row r="49" spans="1:11" s="60" customFormat="1">
+      <c r="A49" s="118" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" s="62" customFormat="1">
-      <c r="A48" s="50">
-        <v>7</v>
-      </c>
-      <c r="B48" s="146" t="s">
-        <v>80</v>
-      </c>
-      <c r="C48" s="147"/>
-      <c r="D48" s="136" t="s">
-        <v>81</v>
-      </c>
-      <c r="E48" s="137"/>
-      <c r="F48" s="136" t="s">
-        <v>82</v>
-      </c>
-      <c r="G48" s="137"/>
-      <c r="H48" s="142" t="s">
+      <c r="B49" s="144"/>
+      <c r="C49" s="145"/>
+      <c r="D49" s="136"/>
+      <c r="E49" s="137"/>
+      <c r="F49" s="136"/>
+      <c r="G49" s="137"/>
+      <c r="H49" s="118" t="s">
+        <v>27</v>
+      </c>
+      <c r="I49" s="118" t="s">
+        <v>1</v>
+      </c>
+      <c r="J49" s="118" t="s">
+        <v>30</v>
+      </c>
+      <c r="K49" s="130"/>
+    </row>
+    <row r="50" spans="1:11" s="60" customFormat="1">
+      <c r="A50" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" s="144"/>
+      <c r="C50" s="145"/>
+      <c r="D50" s="136"/>
+      <c r="E50" s="137"/>
+      <c r="F50" s="136"/>
+      <c r="G50" s="137"/>
+      <c r="H50" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="I50" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="J50" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="K50" s="130"/>
+    </row>
+    <row r="51" spans="1:11" s="60" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A51" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="144"/>
+      <c r="C51" s="145"/>
+      <c r="D51" s="136"/>
+      <c r="E51" s="137"/>
+      <c r="F51" s="136"/>
+      <c r="G51" s="137"/>
+      <c r="H51" s="118" t="s">
         <v>29</v>
       </c>
-      <c r="I48" s="143"/>
-      <c r="J48" s="54" t="s">
-        <v>83</v>
-      </c>
-      <c r="K48" s="133"/>
-    </row>
-    <row r="49" spans="1:11" s="62" customFormat="1">
-      <c r="A49" s="122" t="s">
+      <c r="I51" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="B49" s="148"/>
-      <c r="C49" s="149"/>
-      <c r="D49" s="138"/>
-      <c r="E49" s="139"/>
-      <c r="F49" s="138"/>
-      <c r="G49" s="139"/>
-      <c r="H49" s="122" t="s">
-        <v>28</v>
-      </c>
-      <c r="I49" s="122" t="s">
-        <v>1</v>
-      </c>
-      <c r="J49" s="122" t="s">
-        <v>31</v>
-      </c>
-      <c r="K49" s="134"/>
-    </row>
-    <row r="50" spans="1:11" s="62" customFormat="1">
-      <c r="A50" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="B50" s="148"/>
-      <c r="C50" s="149"/>
-      <c r="D50" s="138"/>
-      <c r="E50" s="139"/>
-      <c r="F50" s="138"/>
-      <c r="G50" s="139"/>
-      <c r="H50" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="I50" s="52" t="s">
-        <v>73</v>
-      </c>
-      <c r="J50" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="K50" s="134"/>
-    </row>
-    <row r="51" spans="1:11" s="62" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A51" s="122" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="148"/>
-      <c r="C51" s="149"/>
-      <c r="D51" s="138"/>
-      <c r="E51" s="139"/>
-      <c r="F51" s="138"/>
-      <c r="G51" s="139"/>
-      <c r="H51" s="122" t="s">
-        <v>30</v>
-      </c>
-      <c r="I51" s="122" t="s">
-        <v>27</v>
-      </c>
-      <c r="J51" s="122"/>
-      <c r="K51" s="134"/>
-    </row>
-    <row r="52" spans="1:11" s="62" customFormat="1">
-      <c r="A52" s="53">
-        <v>823</v>
-      </c>
-      <c r="B52" s="150"/>
-      <c r="C52" s="151"/>
-      <c r="D52" s="140"/>
-      <c r="E52" s="141"/>
-      <c r="F52" s="140"/>
-      <c r="G52" s="141"/>
-      <c r="H52" s="55">
+      <c r="J51" s="118"/>
+      <c r="K51" s="130"/>
+    </row>
+    <row r="52" spans="1:11" s="60" customFormat="1">
+      <c r="A52" s="51">
+        <v>877</v>
+      </c>
+      <c r="B52" s="146"/>
+      <c r="C52" s="147"/>
+      <c r="D52" s="138"/>
+      <c r="E52" s="139"/>
+      <c r="F52" s="138"/>
+      <c r="G52" s="139"/>
+      <c r="H52" s="53">
         <f ca="1">TODAY()</f>
         <v>43443</v>
       </c>
-      <c r="I52" s="52">
+      <c r="I52" s="50">
         <v>43446</v>
       </c>
-      <c r="J52" s="50"/>
-      <c r="K52" s="135"/>
-    </row>
-    <row r="53" spans="1:11" s="62" customFormat="1">
-      <c r="A53" s="123" t="s">
-        <v>20</v>
-      </c>
-      <c r="B53" s="131" t="s">
+      <c r="J52" s="48"/>
+      <c r="K52" s="131"/>
+    </row>
+    <row r="53" spans="1:11" s="60" customFormat="1">
+      <c r="A53" s="119" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="132"/>
-      <c r="D53" s="131" t="s">
-        <v>49</v>
-      </c>
-      <c r="E53" s="132"/>
-      <c r="F53" s="131" t="s">
+      <c r="C53" s="128"/>
+      <c r="D53" s="127" t="s">
+        <v>48</v>
+      </c>
+      <c r="E53" s="128"/>
+      <c r="F53" s="127" t="s">
+        <v>21</v>
+      </c>
+      <c r="G53" s="128"/>
+      <c r="H53" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="G53" s="132"/>
-      <c r="H53" s="152" t="s">
+      <c r="I53" s="148"/>
+      <c r="J53" s="119" t="s">
         <v>23</v>
       </c>
-      <c r="I53" s="152"/>
-      <c r="J53" s="123" t="s">
+      <c r="K53" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="K53" s="123" t="s">
+    </row>
+    <row r="54" spans="1:11" s="60" customFormat="1">
+      <c r="A54" s="48">
+        <v>8</v>
+      </c>
+      <c r="B54" s="142" t="s">
+        <v>83</v>
+      </c>
+      <c r="C54" s="143"/>
+      <c r="D54" s="134" t="s">
+        <v>84</v>
+      </c>
+      <c r="E54" s="135"/>
+      <c r="F54" s="134" t="s">
+        <v>85</v>
+      </c>
+      <c r="G54" s="135"/>
+      <c r="H54" s="132" t="s">
+        <v>31</v>
+      </c>
+      <c r="I54" s="133"/>
+      <c r="J54" s="48"/>
+      <c r="K54" s="129"/>
+    </row>
+    <row r="55" spans="1:11" s="60" customFormat="1">
+      <c r="A55" s="119" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" s="62" customFormat="1">
-      <c r="A54" s="50">
-        <v>8</v>
-      </c>
-      <c r="B54" s="146" t="s">
-        <v>84</v>
-      </c>
-      <c r="C54" s="147"/>
-      <c r="D54" s="136" t="s">
-        <v>85</v>
-      </c>
-      <c r="E54" s="137"/>
-      <c r="F54" s="136" t="s">
-        <v>86</v>
-      </c>
-      <c r="G54" s="137"/>
-      <c r="H54" s="144" t="s">
-        <v>32</v>
-      </c>
-      <c r="I54" s="145"/>
-      <c r="J54" s="50"/>
-      <c r="K54" s="133"/>
-    </row>
-    <row r="55" spans="1:11" s="62" customFormat="1">
-      <c r="A55" s="123" t="s">
-        <v>26</v>
-      </c>
-      <c r="B55" s="148"/>
-      <c r="C55" s="149"/>
-      <c r="D55" s="138"/>
-      <c r="E55" s="139"/>
-      <c r="F55" s="138"/>
-      <c r="G55" s="139"/>
-      <c r="H55" s="123" t="s">
-        <v>28</v>
-      </c>
-      <c r="I55" s="123" t="s">
+      <c r="B55" s="144"/>
+      <c r="C55" s="145"/>
+      <c r="D55" s="136"/>
+      <c r="E55" s="137"/>
+      <c r="F55" s="136"/>
+      <c r="G55" s="137"/>
+      <c r="H55" s="119" t="s">
+        <v>27</v>
+      </c>
+      <c r="I55" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="J55" s="123" t="s">
-        <v>31</v>
-      </c>
-      <c r="K55" s="134"/>
-    </row>
-    <row r="56" spans="1:11" s="62" customFormat="1">
-      <c r="A56" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="B56" s="148"/>
-      <c r="C56" s="149"/>
-      <c r="D56" s="138"/>
-      <c r="E56" s="139"/>
-      <c r="F56" s="138"/>
-      <c r="G56" s="139"/>
-      <c r="H56" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="I56" s="52"/>
-      <c r="J56" s="50"/>
-      <c r="K56" s="134"/>
-    </row>
-    <row r="57" spans="1:11" s="62" customFormat="1" ht="10.5" customHeight="1">
-      <c r="A57" s="123" t="s">
+      <c r="J55" s="119" t="s">
+        <v>30</v>
+      </c>
+      <c r="K55" s="130"/>
+    </row>
+    <row r="56" spans="1:11" s="60" customFormat="1">
+      <c r="A56" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B56" s="144"/>
+      <c r="C56" s="145"/>
+      <c r="D56" s="136"/>
+      <c r="E56" s="137"/>
+      <c r="F56" s="136"/>
+      <c r="G56" s="137"/>
+      <c r="H56" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="I56" s="50"/>
+      <c r="J56" s="48"/>
+      <c r="K56" s="130"/>
+    </row>
+    <row r="57" spans="1:11" s="60" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A57" s="119" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="148"/>
-      <c r="C57" s="149"/>
-      <c r="D57" s="138"/>
-      <c r="E57" s="139"/>
-      <c r="F57" s="138"/>
-      <c r="G57" s="139"/>
-      <c r="H57" s="123" t="s">
-        <v>30</v>
-      </c>
-      <c r="I57" s="123"/>
-      <c r="J57" s="123"/>
-      <c r="K57" s="134"/>
-    </row>
-    <row r="58" spans="1:11" s="62" customFormat="1">
-      <c r="A58" s="53">
-        <v>922</v>
-      </c>
-      <c r="B58" s="150"/>
-      <c r="C58" s="151"/>
-      <c r="D58" s="140"/>
-      <c r="E58" s="141"/>
-      <c r="F58" s="140"/>
-      <c r="G58" s="141"/>
-      <c r="H58" s="55">
+      <c r="B57" s="144"/>
+      <c r="C57" s="145"/>
+      <c r="D57" s="136"/>
+      <c r="E57" s="137"/>
+      <c r="F57" s="136"/>
+      <c r="G57" s="137"/>
+      <c r="H57" s="119" t="s">
+        <v>29</v>
+      </c>
+      <c r="I57" s="119"/>
+      <c r="J57" s="119"/>
+      <c r="K57" s="130"/>
+    </row>
+    <row r="58" spans="1:11" s="60" customFormat="1">
+      <c r="A58" s="51">
+        <v>860</v>
+      </c>
+      <c r="B58" s="146"/>
+      <c r="C58" s="147"/>
+      <c r="D58" s="138"/>
+      <c r="E58" s="139"/>
+      <c r="F58" s="138"/>
+      <c r="G58" s="139"/>
+      <c r="H58" s="53">
         <f ca="1">TODAY()</f>
         <v>43443</v>
       </c>
-      <c r="I58" s="52"/>
-      <c r="J58" s="50"/>
-      <c r="K58" s="135"/>
-    </row>
-    <row r="59" spans="1:11" s="62" customFormat="1">
-      <c r="A59" s="122" t="s">
+      <c r="I58" s="50"/>
+      <c r="J58" s="48"/>
+      <c r="K58" s="131"/>
+    </row>
+    <row r="59" spans="1:11" s="60" customFormat="1">
+      <c r="A59" s="118" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="125" t="s">
         <v>20</v>
       </c>
-      <c r="B59" s="129" t="s">
+      <c r="C59" s="126"/>
+      <c r="D59" s="125" t="s">
+        <v>48</v>
+      </c>
+      <c r="E59" s="126"/>
+      <c r="F59" s="125" t="s">
         <v>21</v>
       </c>
-      <c r="C59" s="130"/>
-      <c r="D59" s="129" t="s">
-        <v>49</v>
-      </c>
-      <c r="E59" s="130"/>
-      <c r="F59" s="129" t="s">
+      <c r="G59" s="126"/>
+      <c r="H59" s="123" t="s">
         <v>22</v>
       </c>
-      <c r="G59" s="130"/>
-      <c r="H59" s="127" t="s">
+      <c r="I59" s="123"/>
+      <c r="J59" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="I59" s="127"/>
-      <c r="J59" s="122" t="s">
+      <c r="K59" s="117" t="s">
         <v>24</v>
       </c>
-      <c r="K59" s="121" t="s">
+    </row>
+    <row r="60" spans="1:11" s="60" customFormat="1">
+      <c r="A60" s="48">
+        <v>9</v>
+      </c>
+      <c r="B60" s="142" t="s">
+        <v>86</v>
+      </c>
+      <c r="C60" s="143"/>
+      <c r="D60" s="134" t="s">
+        <v>87</v>
+      </c>
+      <c r="E60" s="135"/>
+      <c r="F60" s="134" t="s">
+        <v>88</v>
+      </c>
+      <c r="G60" s="135"/>
+      <c r="H60" s="140" t="s">
+        <v>31</v>
+      </c>
+      <c r="I60" s="141"/>
+      <c r="J60" s="52"/>
+      <c r="K60" s="129"/>
+    </row>
+    <row r="61" spans="1:11" s="60" customFormat="1">
+      <c r="A61" s="118" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" s="62" customFormat="1">
-      <c r="A60" s="50">
-        <v>9</v>
-      </c>
-      <c r="B60" s="146" t="s">
-        <v>87</v>
-      </c>
-      <c r="C60" s="147"/>
-      <c r="D60" s="136" t="s">
-        <v>88</v>
-      </c>
-      <c r="E60" s="137"/>
-      <c r="F60" s="136" t="s">
-        <v>89</v>
-      </c>
-      <c r="G60" s="137"/>
-      <c r="H60" s="142" t="s">
-        <v>32</v>
-      </c>
-      <c r="I60" s="143"/>
-      <c r="J60" s="54"/>
-      <c r="K60" s="133"/>
-    </row>
-    <row r="61" spans="1:11" s="62" customFormat="1">
-      <c r="A61" s="122" t="s">
+      <c r="B61" s="144"/>
+      <c r="C61" s="145"/>
+      <c r="D61" s="136"/>
+      <c r="E61" s="137"/>
+      <c r="F61" s="136"/>
+      <c r="G61" s="137"/>
+      <c r="H61" s="118" t="s">
+        <v>27</v>
+      </c>
+      <c r="I61" s="118" t="s">
+        <v>1</v>
+      </c>
+      <c r="J61" s="118" t="s">
+        <v>30</v>
+      </c>
+      <c r="K61" s="130"/>
+    </row>
+    <row r="62" spans="1:11" s="60" customFormat="1">
+      <c r="A62" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B62" s="144"/>
+      <c r="C62" s="145"/>
+      <c r="D62" s="136"/>
+      <c r="E62" s="137"/>
+      <c r="F62" s="136"/>
+      <c r="G62" s="137"/>
+      <c r="H62" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="I62" s="50"/>
+      <c r="J62" s="48"/>
+      <c r="K62" s="130"/>
+    </row>
+    <row r="63" spans="1:11" s="60" customFormat="1">
+      <c r="A63" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="144"/>
+      <c r="C63" s="145"/>
+      <c r="D63" s="136"/>
+      <c r="E63" s="137"/>
+      <c r="F63" s="136"/>
+      <c r="G63" s="137"/>
+      <c r="H63" s="118" t="s">
+        <v>29</v>
+      </c>
+      <c r="I63" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="B61" s="148"/>
-      <c r="C61" s="149"/>
-      <c r="D61" s="138"/>
-      <c r="E61" s="139"/>
-      <c r="F61" s="138"/>
-      <c r="G61" s="139"/>
-      <c r="H61" s="122" t="s">
-        <v>28</v>
-      </c>
-      <c r="I61" s="122" t="s">
-        <v>1</v>
-      </c>
-      <c r="J61" s="122" t="s">
-        <v>31</v>
-      </c>
-      <c r="K61" s="134"/>
-    </row>
-    <row r="62" spans="1:11" s="62" customFormat="1">
-      <c r="A62" s="51" t="s">
-        <v>99</v>
-      </c>
-      <c r="B62" s="148"/>
-      <c r="C62" s="149"/>
-      <c r="D62" s="138"/>
-      <c r="E62" s="139"/>
-      <c r="F62" s="138"/>
-      <c r="G62" s="139"/>
-      <c r="H62" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="I62" s="52"/>
-      <c r="J62" s="50"/>
-      <c r="K62" s="134"/>
-    </row>
-    <row r="63" spans="1:11" s="62" customFormat="1">
-      <c r="A63" s="122" t="s">
-        <v>0</v>
-      </c>
-      <c r="B63" s="148"/>
-      <c r="C63" s="149"/>
-      <c r="D63" s="138"/>
-      <c r="E63" s="139"/>
-      <c r="F63" s="138"/>
-      <c r="G63" s="139"/>
-      <c r="H63" s="122" t="s">
-        <v>30</v>
-      </c>
-      <c r="I63" s="122" t="s">
-        <v>27</v>
-      </c>
-      <c r="J63" s="122"/>
-      <c r="K63" s="134"/>
-    </row>
-    <row r="64" spans="1:11" s="62" customFormat="1">
-      <c r="A64" s="53">
-        <v>823</v>
-      </c>
-      <c r="B64" s="150"/>
-      <c r="C64" s="151"/>
-      <c r="D64" s="140"/>
-      <c r="E64" s="141"/>
-      <c r="F64" s="140"/>
-      <c r="G64" s="141"/>
-      <c r="H64" s="55">
+      <c r="J63" s="118"/>
+      <c r="K63" s="130"/>
+    </row>
+    <row r="64" spans="1:11" s="60" customFormat="1">
+      <c r="A64" s="51">
+        <v>907</v>
+      </c>
+      <c r="B64" s="146"/>
+      <c r="C64" s="147"/>
+      <c r="D64" s="138"/>
+      <c r="E64" s="139"/>
+      <c r="F64" s="138"/>
+      <c r="G64" s="139"/>
+      <c r="H64" s="53">
         <f ca="1">TODAY()</f>
         <v>43443</v>
       </c>
-      <c r="I64" s="52"/>
-      <c r="J64" s="50"/>
-      <c r="K64" s="135"/>
-    </row>
-    <row r="65" spans="1:11" s="62" customFormat="1">
-      <c r="A65" s="103" t="s">
+      <c r="I64" s="50"/>
+      <c r="J64" s="48"/>
+      <c r="K64" s="131"/>
+    </row>
+    <row r="65" spans="1:11" s="60" customFormat="1">
+      <c r="A65" s="101" t="s">
+        <v>99</v>
+      </c>
+      <c r="B65" s="122" t="s">
+        <v>90</v>
+      </c>
+      <c r="C65" s="122"/>
+      <c r="D65" s="122"/>
+      <c r="E65" s="122"/>
+      <c r="F65" s="122"/>
+      <c r="G65" s="122"/>
+      <c r="H65" s="122"/>
+      <c r="I65" s="122"/>
+      <c r="J65" s="122"/>
+      <c r="K65" s="122"/>
+    </row>
+    <row r="66" spans="1:11" s="60" customFormat="1">
+      <c r="A66" s="119" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" s="127" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" s="128"/>
+      <c r="D66" s="127" t="s">
+        <v>48</v>
+      </c>
+      <c r="E66" s="128"/>
+      <c r="F66" s="127" t="s">
+        <v>21</v>
+      </c>
+      <c r="G66" s="128"/>
+      <c r="H66" s="148" t="s">
+        <v>22</v>
+      </c>
+      <c r="I66" s="148"/>
+      <c r="J66" s="119" t="s">
+        <v>23</v>
+      </c>
+      <c r="K66" s="119" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" s="60" customFormat="1">
+      <c r="A67" s="48">
+        <v>10</v>
+      </c>
+      <c r="B67" s="142" t="s">
+        <v>91</v>
+      </c>
+      <c r="C67" s="143"/>
+      <c r="D67" s="134" t="s">
+        <v>92</v>
+      </c>
+      <c r="E67" s="135"/>
+      <c r="F67" s="134" t="s">
+        <v>93</v>
+      </c>
+      <c r="G67" s="135"/>
+      <c r="H67" s="132" t="s">
+        <v>31</v>
+      </c>
+      <c r="I67" s="133"/>
+      <c r="J67" s="48"/>
+      <c r="K67" s="129"/>
+    </row>
+    <row r="68" spans="1:11" s="60" customFormat="1">
+      <c r="A68" s="119" t="s">
+        <v>25</v>
+      </c>
+      <c r="B68" s="144"/>
+      <c r="C68" s="145"/>
+      <c r="D68" s="136"/>
+      <c r="E68" s="137"/>
+      <c r="F68" s="136"/>
+      <c r="G68" s="137"/>
+      <c r="H68" s="119" t="s">
+        <v>27</v>
+      </c>
+      <c r="I68" s="119" t="s">
+        <v>1</v>
+      </c>
+      <c r="J68" s="119" t="s">
+        <v>30</v>
+      </c>
+      <c r="K68" s="130"/>
+    </row>
+    <row r="69" spans="1:11" s="60" customFormat="1">
+      <c r="A69" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="B65" s="126" t="s">
-        <v>91</v>
-      </c>
-      <c r="C65" s="126"/>
-      <c r="D65" s="126"/>
-      <c r="E65" s="126"/>
-      <c r="F65" s="126"/>
-      <c r="G65" s="126"/>
-      <c r="H65" s="126"/>
-      <c r="I65" s="126"/>
-      <c r="J65" s="126"/>
-      <c r="K65" s="126"/>
-    </row>
-    <row r="66" spans="1:11" s="62" customFormat="1">
-      <c r="A66" s="123" t="s">
-        <v>20</v>
-      </c>
-      <c r="B66" s="131" t="s">
-        <v>2</v>
-      </c>
-      <c r="C66" s="132"/>
-      <c r="D66" s="131" t="s">
-        <v>49</v>
-      </c>
-      <c r="E66" s="132"/>
-      <c r="F66" s="131" t="s">
-        <v>22</v>
-      </c>
-      <c r="G66" s="132"/>
-      <c r="H66" s="152" t="s">
-        <v>23</v>
-      </c>
-      <c r="I66" s="152"/>
-      <c r="J66" s="123" t="s">
-        <v>24</v>
-      </c>
-      <c r="K66" s="123" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" s="62" customFormat="1">
-      <c r="A67" s="50">
-        <v>10</v>
-      </c>
-      <c r="B67" s="146" t="s">
-        <v>92</v>
-      </c>
-      <c r="C67" s="147"/>
-      <c r="D67" s="136" t="s">
-        <v>93</v>
-      </c>
-      <c r="E67" s="137"/>
-      <c r="F67" s="136" t="s">
-        <v>94</v>
-      </c>
-      <c r="G67" s="137"/>
-      <c r="H67" s="144" t="s">
-        <v>32</v>
-      </c>
-      <c r="I67" s="145"/>
-      <c r="J67" s="50"/>
-      <c r="K67" s="133"/>
-    </row>
-    <row r="68" spans="1:11" s="62" customFormat="1">
-      <c r="A68" s="123" t="s">
-        <v>26</v>
-      </c>
-      <c r="B68" s="148"/>
-      <c r="C68" s="149"/>
-      <c r="D68" s="138"/>
-      <c r="E68" s="139"/>
-      <c r="F68" s="138"/>
-      <c r="G68" s="139"/>
-      <c r="H68" s="123" t="s">
-        <v>28</v>
-      </c>
-      <c r="I68" s="123" t="s">
-        <v>1</v>
-      </c>
-      <c r="J68" s="123" t="s">
-        <v>31</v>
-      </c>
-      <c r="K68" s="134"/>
-    </row>
-    <row r="69" spans="1:11" s="62" customFormat="1">
-      <c r="A69" s="51" t="s">
-        <v>101</v>
-      </c>
-      <c r="B69" s="148"/>
-      <c r="C69" s="149"/>
-      <c r="D69" s="138"/>
-      <c r="E69" s="139"/>
-      <c r="F69" s="138"/>
-      <c r="G69" s="139"/>
-      <c r="H69" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="I69" s="52"/>
-      <c r="J69" s="50"/>
-      <c r="K69" s="134"/>
-    </row>
-    <row r="70" spans="1:11" s="62" customFormat="1">
-      <c r="A70" s="123" t="s">
+      <c r="B69" s="144"/>
+      <c r="C69" s="145"/>
+      <c r="D69" s="136"/>
+      <c r="E69" s="137"/>
+      <c r="F69" s="136"/>
+      <c r="G69" s="137"/>
+      <c r="H69" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="I69" s="50"/>
+      <c r="J69" s="48"/>
+      <c r="K69" s="130"/>
+    </row>
+    <row r="70" spans="1:11" s="60" customFormat="1">
+      <c r="A70" s="119" t="s">
         <v>0</v>
       </c>
-      <c r="B70" s="148"/>
-      <c r="C70" s="149"/>
-      <c r="D70" s="138"/>
-      <c r="E70" s="139"/>
-      <c r="F70" s="138"/>
-      <c r="G70" s="139"/>
-      <c r="H70" s="123" t="s">
-        <v>30</v>
-      </c>
-      <c r="I70" s="123"/>
-      <c r="J70" s="123"/>
-      <c r="K70" s="134"/>
-    </row>
-    <row r="71" spans="1:11" s="62" customFormat="1">
-      <c r="A71" s="53">
-        <v>922</v>
-      </c>
-      <c r="B71" s="150"/>
-      <c r="C71" s="151"/>
-      <c r="D71" s="140"/>
-      <c r="E71" s="141"/>
-      <c r="F71" s="140"/>
-      <c r="G71" s="141"/>
-      <c r="H71" s="55">
+      <c r="B70" s="144"/>
+      <c r="C70" s="145"/>
+      <c r="D70" s="136"/>
+      <c r="E70" s="137"/>
+      <c r="F70" s="136"/>
+      <c r="G70" s="137"/>
+      <c r="H70" s="119" t="s">
+        <v>29</v>
+      </c>
+      <c r="I70" s="119"/>
+      <c r="J70" s="119"/>
+      <c r="K70" s="130"/>
+    </row>
+    <row r="71" spans="1:11" s="60" customFormat="1">
+      <c r="A71" s="51">
+        <v>457</v>
+      </c>
+      <c r="B71" s="146"/>
+      <c r="C71" s="147"/>
+      <c r="D71" s="138"/>
+      <c r="E71" s="139"/>
+      <c r="F71" s="138"/>
+      <c r="G71" s="139"/>
+      <c r="H71" s="53">
         <f ca="1">TODAY()</f>
         <v>43443</v>
       </c>
-      <c r="I71" s="52"/>
-      <c r="J71" s="50"/>
-      <c r="K71" s="135"/>
-    </row>
-    <row r="72" spans="1:11" s="62" customFormat="1">
-      <c r="A72" s="66"/>
-      <c r="H72" s="66"/>
-      <c r="I72" s="66"/>
-      <c r="J72" s="66"/>
-      <c r="K72" s="66"/>
-    </row>
-    <row r="73" spans="1:11" s="62" customFormat="1">
-      <c r="A73" s="66"/>
-      <c r="H73" s="66"/>
-      <c r="I73" s="66"/>
-      <c r="J73" s="66"/>
-      <c r="K73" s="66"/>
-    </row>
-    <row r="74" spans="1:11" s="62" customFormat="1">
-      <c r="A74" s="66"/>
-      <c r="H74" s="66"/>
-      <c r="I74" s="66"/>
-      <c r="J74" s="66"/>
-      <c r="K74" s="66"/>
-    </row>
-    <row r="75" spans="1:11" s="62" customFormat="1">
-      <c r="A75" s="66"/>
-      <c r="H75" s="66"/>
-      <c r="I75" s="66"/>
-      <c r="J75" s="66"/>
-      <c r="K75" s="66"/>
-    </row>
-    <row r="76" spans="1:11" s="62" customFormat="1">
-      <c r="A76" s="66"/>
-      <c r="H76" s="66"/>
-      <c r="I76" s="66"/>
-      <c r="J76" s="66"/>
-      <c r="K76" s="66"/>
-    </row>
-    <row r="77" spans="1:11" s="62" customFormat="1">
-      <c r="A77" s="66"/>
-      <c r="H77" s="66"/>
-      <c r="I77" s="66"/>
-      <c r="J77" s="66"/>
-      <c r="K77" s="66"/>
-    </row>
-    <row r="78" spans="1:11" s="62" customFormat="1">
-      <c r="A78" s="66"/>
-      <c r="H78" s="66"/>
-      <c r="I78" s="66"/>
-      <c r="J78" s="66"/>
-      <c r="K78" s="66"/>
-    </row>
-    <row r="79" spans="1:11" s="62" customFormat="1">
-      <c r="A79" s="66"/>
-      <c r="H79" s="66"/>
-      <c r="I79" s="66"/>
-      <c r="J79" s="66"/>
-      <c r="K79" s="66"/>
-    </row>
-    <row r="80" spans="1:11" s="62" customFormat="1">
-      <c r="A80" s="66"/>
-      <c r="H80" s="66"/>
-      <c r="I80" s="66"/>
-      <c r="J80" s="66"/>
-      <c r="K80" s="66"/>
-    </row>
-    <row r="81" spans="1:11" s="62" customFormat="1">
-      <c r="A81" s="66"/>
-      <c r="H81" s="66"/>
-      <c r="I81" s="66"/>
-      <c r="J81" s="66"/>
-      <c r="K81" s="66"/>
-    </row>
-    <row r="82" spans="1:11" s="62" customFormat="1">
-      <c r="A82" s="66"/>
-      <c r="H82" s="66"/>
-      <c r="I82" s="66"/>
-      <c r="J82" s="66"/>
-      <c r="K82" s="66"/>
-    </row>
-    <row r="83" spans="1:11" s="62" customFormat="1">
-      <c r="A83" s="66"/>
-      <c r="H83" s="66"/>
-      <c r="I83" s="66"/>
-      <c r="J83" s="66"/>
-      <c r="K83" s="66"/>
-    </row>
-    <row r="84" spans="1:11" s="62" customFormat="1">
-      <c r="A84" s="66"/>
-      <c r="H84" s="66"/>
-      <c r="I84" s="66"/>
-      <c r="J84" s="66"/>
-      <c r="K84" s="66"/>
-    </row>
-    <row r="85" spans="1:11" s="62" customFormat="1">
-      <c r="A85" s="66"/>
-      <c r="H85" s="66"/>
-      <c r="I85" s="66"/>
-      <c r="J85" s="66"/>
-      <c r="K85" s="66"/>
-    </row>
-    <row r="86" spans="1:11" s="62" customFormat="1">
-      <c r="A86" s="66"/>
-      <c r="H86" s="66"/>
-      <c r="I86" s="66"/>
-      <c r="J86" s="66"/>
-      <c r="K86" s="66"/>
-    </row>
-    <row r="87" spans="1:11" s="62" customFormat="1">
-      <c r="A87" s="66"/>
-      <c r="H87" s="66"/>
-      <c r="I87" s="66"/>
-      <c r="J87" s="66"/>
-      <c r="K87" s="66"/>
-    </row>
-    <row r="88" spans="1:11" s="62" customFormat="1">
-      <c r="A88" s="66"/>
-      <c r="H88" s="66"/>
-      <c r="I88" s="66"/>
-      <c r="J88" s="66"/>
-      <c r="K88" s="66"/>
-    </row>
-    <row r="89" spans="1:11" s="62" customFormat="1">
+      <c r="I71" s="50"/>
+      <c r="J71" s="48"/>
+      <c r="K71" s="131"/>
+    </row>
+    <row r="72" spans="1:11" s="60" customFormat="1">
+      <c r="A72" s="64"/>
+      <c r="H72" s="64"/>
+      <c r="I72" s="64"/>
+      <c r="J72" s="64"/>
+      <c r="K72" s="64"/>
+    </row>
+    <row r="73" spans="1:11" s="60" customFormat="1">
+      <c r="A73" s="64"/>
+      <c r="H73" s="64"/>
+      <c r="I73" s="64"/>
+      <c r="J73" s="64"/>
+      <c r="K73" s="64"/>
+    </row>
+    <row r="74" spans="1:11" s="60" customFormat="1">
+      <c r="A74" s="64"/>
+      <c r="H74" s="64"/>
+      <c r="I74" s="64"/>
+      <c r="J74" s="64"/>
+      <c r="K74" s="64"/>
+    </row>
+    <row r="75" spans="1:11" s="60" customFormat="1">
+      <c r="A75" s="64"/>
+      <c r="H75" s="64"/>
+      <c r="I75" s="64"/>
+      <c r="J75" s="64"/>
+      <c r="K75" s="64"/>
+    </row>
+    <row r="76" spans="1:11" s="60" customFormat="1">
+      <c r="A76" s="64"/>
+      <c r="H76" s="64"/>
+      <c r="I76" s="64"/>
+      <c r="J76" s="64"/>
+      <c r="K76" s="64"/>
+    </row>
+    <row r="77" spans="1:11" s="60" customFormat="1">
+      <c r="A77" s="64"/>
+      <c r="H77" s="64"/>
+      <c r="I77" s="64"/>
+      <c r="J77" s="64"/>
+      <c r="K77" s="64"/>
+    </row>
+    <row r="78" spans="1:11" s="60" customFormat="1">
+      <c r="A78" s="64"/>
+      <c r="H78" s="64"/>
+      <c r="I78" s="64"/>
+      <c r="J78" s="64"/>
+      <c r="K78" s="64"/>
+    </row>
+    <row r="79" spans="1:11" s="60" customFormat="1">
+      <c r="A79" s="64"/>
+      <c r="H79" s="64"/>
+      <c r="I79" s="64"/>
+      <c r="J79" s="64"/>
+      <c r="K79" s="64"/>
+    </row>
+    <row r="80" spans="1:11" s="60" customFormat="1">
+      <c r="A80" s="64"/>
+      <c r="H80" s="64"/>
+      <c r="I80" s="64"/>
+      <c r="J80" s="64"/>
+      <c r="K80" s="64"/>
+    </row>
+    <row r="81" spans="1:11" s="60" customFormat="1">
+      <c r="A81" s="64"/>
+      <c r="H81" s="64"/>
+      <c r="I81" s="64"/>
+      <c r="J81" s="64"/>
+      <c r="K81" s="64"/>
+    </row>
+    <row r="82" spans="1:11" s="60" customFormat="1">
+      <c r="A82" s="64"/>
+      <c r="H82" s="64"/>
+      <c r="I82" s="64"/>
+      <c r="J82" s="64"/>
+      <c r="K82" s="64"/>
+    </row>
+    <row r="83" spans="1:11" s="60" customFormat="1">
+      <c r="A83" s="64"/>
+      <c r="H83" s="64"/>
+      <c r="I83" s="64"/>
+      <c r="J83" s="64"/>
+      <c r="K83" s="64"/>
+    </row>
+    <row r="84" spans="1:11" s="60" customFormat="1">
+      <c r="A84" s="64"/>
+      <c r="H84" s="64"/>
+      <c r="I84" s="64"/>
+      <c r="J84" s="64"/>
+      <c r="K84" s="64"/>
+    </row>
+    <row r="85" spans="1:11" s="60" customFormat="1">
+      <c r="A85" s="64"/>
+      <c r="H85" s="64"/>
+      <c r="I85" s="64"/>
+      <c r="J85" s="64"/>
+      <c r="K85" s="64"/>
+    </row>
+    <row r="86" spans="1:11" s="60" customFormat="1">
+      <c r="A86" s="64"/>
+      <c r="H86" s="64"/>
+      <c r="I86" s="64"/>
+      <c r="J86" s="64"/>
+      <c r="K86" s="64"/>
+    </row>
+    <row r="87" spans="1:11" s="60" customFormat="1">
+      <c r="A87" s="64"/>
+      <c r="H87" s="64"/>
+      <c r="I87" s="64"/>
+      <c r="J87" s="64"/>
+      <c r="K87" s="64"/>
+    </row>
+    <row r="88" spans="1:11" s="60" customFormat="1">
+      <c r="A88" s="64"/>
+      <c r="H88" s="64"/>
+      <c r="I88" s="64"/>
+      <c r="J88" s="64"/>
+      <c r="K88" s="64"/>
+    </row>
+    <row r="89" spans="1:11" s="60" customFormat="1">
       <c r="A89" s="2"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -4901,7 +4891,7 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="1:11" s="62" customFormat="1">
+    <row r="90" spans="1:11" s="60" customFormat="1">
       <c r="A90" s="2"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -4914,7 +4904,7 @@
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
     </row>
-    <row r="91" spans="1:11" s="62" customFormat="1">
+    <row r="91" spans="1:11" s="60" customFormat="1">
       <c r="A91" s="2"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -4927,7 +4917,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="1:11" s="62" customFormat="1">
+    <row r="92" spans="1:11" s="60" customFormat="1">
       <c r="A92" s="2"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -4940,7 +4930,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" s="62" customFormat="1">
+    <row r="93" spans="1:11" s="60" customFormat="1">
       <c r="A93" s="2"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -4953,7 +4943,7 @@
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
     </row>
-    <row r="94" spans="1:11" s="62" customFormat="1">
+    <row r="94" spans="1:11" s="60" customFormat="1">
       <c r="A94" s="2"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -4966,7 +4956,7 @@
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
     </row>
-    <row r="95" spans="1:11" s="62" customFormat="1">
+    <row r="95" spans="1:11" s="60" customFormat="1">
       <c r="A95" s="2"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -4979,7 +4969,7 @@
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
     </row>
-    <row r="96" spans="1:11" s="62" customFormat="1">
+    <row r="96" spans="1:11" s="60" customFormat="1">
       <c r="A96" s="2"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -4994,6 +4984,8 @@
     </row>
   </sheetData>
   <mergeCells count="95">
+    <mergeCell ref="K60:K64"/>
+    <mergeCell ref="B65:K65"/>
     <mergeCell ref="K67:K71"/>
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="D66:E66"/>
@@ -5003,34 +4995,26 @@
     <mergeCell ref="D67:E71"/>
     <mergeCell ref="F67:G71"/>
     <mergeCell ref="H67:I67"/>
-    <mergeCell ref="D60:E64"/>
-    <mergeCell ref="F60:G64"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="K60:K64"/>
-    <mergeCell ref="B65:K65"/>
+    <mergeCell ref="K48:K52"/>
     <mergeCell ref="B46:K46"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="F47:G47"/>
     <mergeCell ref="H47:I47"/>
+    <mergeCell ref="F54:G58"/>
+    <mergeCell ref="H54:I54"/>
     <mergeCell ref="B48:C52"/>
     <mergeCell ref="D48:E52"/>
     <mergeCell ref="F48:G52"/>
     <mergeCell ref="H48:I48"/>
-    <mergeCell ref="K48:K52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="B54:C58"/>
-    <mergeCell ref="D54:E58"/>
-    <mergeCell ref="F54:G58"/>
-    <mergeCell ref="H54:I54"/>
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="F59:G59"/>
     <mergeCell ref="H59:I59"/>
     <mergeCell ref="B60:C64"/>
+    <mergeCell ref="D60:E64"/>
+    <mergeCell ref="F60:G64"/>
+    <mergeCell ref="H60:I60"/>
     <mergeCell ref="K54:K58"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="D40:E40"/>
@@ -5041,6 +5025,12 @@
     <mergeCell ref="H41:I41"/>
     <mergeCell ref="K41:K45"/>
     <mergeCell ref="H40:I40"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="B54:C58"/>
+    <mergeCell ref="D54:E58"/>
     <mergeCell ref="B35:C39"/>
     <mergeCell ref="D35:E39"/>
     <mergeCell ref="F35:G39"/>

</xml_diff>